<commit_message>
data preparation for stacked bar chart
</commit_message>
<xml_diff>
--- a/data-cleaning/cleaned.xlsx
+++ b/data-cleaning/cleaned.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1496" uniqueCount="116">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1849" uniqueCount="104">
   <si>
     <t>sexe</t>
   </si>
@@ -193,6 +193,15 @@
     <t>1 fois par mois</t>
   </si>
   <si>
+    <t>rarement</t>
+  </si>
+  <si>
+    <t>occasionnellement</t>
+  </si>
+  <si>
+    <t>Fréquente</t>
+  </si>
+  <si>
     <t>Huile végétale</t>
   </si>
   <si>
@@ -304,64 +313,19 @@
     <t>1</t>
   </si>
   <si>
-    <t>Asm</t>
-  </si>
-  <si>
-    <t>Diabète</t>
-  </si>
-  <si>
-    <t>القلب</t>
-  </si>
-  <si>
-    <t xml:space="preserve">La tension </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Diabète </t>
+    <t>autres</t>
+  </si>
+  <si>
+    <t>aucune maladie</t>
+  </si>
+  <si>
+    <t>diabete</t>
   </si>
   <si>
     <t>HTA</t>
   </si>
   <si>
-    <t>Diabète.. la tention</t>
-  </si>
-  <si>
-    <t>la tension,Insuffisance rénale</t>
-  </si>
-  <si>
-    <t xml:space="preserve">diabétique et asmatique </t>
-  </si>
-  <si>
-    <t>mon père</t>
-  </si>
-  <si>
-    <t>la tension(HTA)</t>
-  </si>
-  <si>
-    <t>Hta</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Diabete rension... </t>
-  </si>
-  <si>
-    <t>diabete</t>
-  </si>
-  <si>
-    <t>Diabete et hta</t>
-  </si>
-  <si>
-    <t xml:space="preserve">les 3 </t>
-  </si>
-  <si>
-    <t>Diabète, tension, ...</t>
-  </si>
-  <si>
-    <t>asthmatique</t>
-  </si>
-  <si>
-    <t>les trois</t>
-  </si>
-  <si>
-    <t>Maladies cardiaques</t>
+    <t>asthme</t>
   </si>
 </sst>
 </file>
@@ -818,17 +782,17 @@
       <c r="K2" t="s">
         <v>51</v>
       </c>
-      <c r="M2">
-        <v>0</v>
-      </c>
-      <c r="N2">
-        <v>3</v>
+      <c r="M2" t="s">
+        <v>59</v>
+      </c>
+      <c r="N2" t="s">
+        <v>60</v>
       </c>
       <c r="O2" t="s">
-        <v>59</v>
-      </c>
-      <c r="P2">
-        <v>5</v>
+        <v>62</v>
+      </c>
+      <c r="P2" t="s">
+        <v>61</v>
       </c>
       <c r="Q2" t="s">
         <v>56</v>
@@ -846,13 +810,13 @@
         <v>56</v>
       </c>
       <c r="V2" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
       <c r="W2" t="s">
         <v>52</v>
       </c>
       <c r="X2" t="s">
-        <v>96</v>
+        <v>99</v>
       </c>
     </row>
     <row r="3" spans="1:24">
@@ -886,17 +850,17 @@
       <c r="K3" t="s">
         <v>51</v>
       </c>
-      <c r="M3">
-        <v>3</v>
-      </c>
-      <c r="N3">
-        <v>5</v>
+      <c r="M3" t="s">
+        <v>60</v>
+      </c>
+      <c r="N3" t="s">
+        <v>61</v>
       </c>
       <c r="O3" t="s">
-        <v>59</v>
-      </c>
-      <c r="P3">
-        <v>3</v>
+        <v>62</v>
+      </c>
+      <c r="P3" t="s">
+        <v>60</v>
       </c>
       <c r="Q3" t="s">
         <v>52</v>
@@ -914,10 +878,13 @@
         <v>52</v>
       </c>
       <c r="V3" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
       <c r="W3" t="s">
         <v>56</v>
+      </c>
+      <c r="X3" t="s">
+        <v>100</v>
       </c>
     </row>
     <row r="4" spans="1:24">
@@ -948,17 +915,17 @@
       <c r="K4" t="s">
         <v>51</v>
       </c>
-      <c r="M4">
-        <v>5</v>
-      </c>
-      <c r="N4">
-        <v>5</v>
+      <c r="M4" t="s">
+        <v>61</v>
+      </c>
+      <c r="N4" t="s">
+        <v>61</v>
       </c>
       <c r="O4" t="s">
-        <v>59</v>
-      </c>
-      <c r="P4">
-        <v>5</v>
+        <v>62</v>
+      </c>
+      <c r="P4" t="s">
+        <v>61</v>
       </c>
       <c r="Q4" t="s">
         <v>56</v>
@@ -976,13 +943,13 @@
         <v>56</v>
       </c>
       <c r="V4" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
       <c r="W4" t="s">
         <v>52</v>
       </c>
       <c r="X4" t="s">
-        <v>97</v>
+        <v>101</v>
       </c>
     </row>
     <row r="5" spans="1:24">
@@ -1016,17 +983,17 @@
       <c r="K5" t="s">
         <v>51</v>
       </c>
-      <c r="M5">
-        <v>3</v>
-      </c>
-      <c r="N5">
-        <v>5</v>
+      <c r="M5" t="s">
+        <v>60</v>
+      </c>
+      <c r="N5" t="s">
+        <v>61</v>
       </c>
       <c r="O5" t="s">
+        <v>62</v>
+      </c>
+      <c r="P5" t="s">
         <v>59</v>
-      </c>
-      <c r="P5">
-        <v>1</v>
       </c>
       <c r="Q5" t="s">
         <v>56</v>
@@ -1044,10 +1011,13 @@
         <v>56</v>
       </c>
       <c r="V5" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
       <c r="W5" t="s">
         <v>56</v>
+      </c>
+      <c r="X5" t="s">
+        <v>100</v>
       </c>
     </row>
     <row r="6" spans="1:24">
@@ -1072,17 +1042,17 @@
       <c r="K6" t="s">
         <v>51</v>
       </c>
-      <c r="M6">
-        <v>2</v>
-      </c>
-      <c r="N6">
-        <v>4</v>
+      <c r="M6" t="s">
+        <v>60</v>
+      </c>
+      <c r="N6" t="s">
+        <v>61</v>
       </c>
       <c r="O6" t="s">
-        <v>60</v>
-      </c>
-      <c r="P6">
-        <v>2</v>
+        <v>63</v>
+      </c>
+      <c r="P6" t="s">
+        <v>60</v>
       </c>
       <c r="Q6" t="s">
         <v>56</v>
@@ -1100,10 +1070,13 @@
         <v>52</v>
       </c>
       <c r="V6" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
       <c r="W6" t="s">
         <v>56</v>
+      </c>
+      <c r="X6" t="s">
+        <v>100</v>
       </c>
     </row>
     <row r="7" spans="1:24">
@@ -1125,17 +1098,17 @@
       <c r="K7" t="s">
         <v>51</v>
       </c>
-      <c r="M7">
-        <v>5</v>
-      </c>
-      <c r="N7">
-        <v>5</v>
+      <c r="M7" t="s">
+        <v>61</v>
+      </c>
+      <c r="N7" t="s">
+        <v>61</v>
       </c>
       <c r="O7" t="s">
+        <v>62</v>
+      </c>
+      <c r="P7" t="s">
         <v>59</v>
-      </c>
-      <c r="P7">
-        <v>0</v>
       </c>
       <c r="Q7" t="s">
         <v>56</v>
@@ -1153,13 +1126,13 @@
         <v>56</v>
       </c>
       <c r="V7" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="W7" t="s">
         <v>52</v>
       </c>
       <c r="X7" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
     </row>
     <row r="8" spans="1:24">
@@ -1181,17 +1154,17 @@
       <c r="K8" t="s">
         <v>51</v>
       </c>
-      <c r="M8">
-        <v>2</v>
-      </c>
-      <c r="N8">
-        <v>3</v>
+      <c r="M8" t="s">
+        <v>60</v>
+      </c>
+      <c r="N8" t="s">
+        <v>60</v>
       </c>
       <c r="O8" t="s">
-        <v>61</v>
-      </c>
-      <c r="P8">
-        <v>2</v>
+        <v>64</v>
+      </c>
+      <c r="P8" t="s">
+        <v>60</v>
       </c>
       <c r="Q8" t="s">
         <v>56</v>
@@ -1213,6 +1186,9 @@
       </c>
       <c r="W8" t="s">
         <v>56</v>
+      </c>
+      <c r="X8" t="s">
+        <v>100</v>
       </c>
     </row>
     <row r="9" spans="1:24">
@@ -1240,17 +1216,17 @@
       <c r="L9" t="s">
         <v>57</v>
       </c>
-      <c r="M9">
-        <v>3</v>
-      </c>
-      <c r="N9">
-        <v>5</v>
+      <c r="M9" t="s">
+        <v>60</v>
+      </c>
+      <c r="N9" t="s">
+        <v>61</v>
       </c>
       <c r="O9" t="s">
-        <v>59</v>
-      </c>
-      <c r="P9">
-        <v>2</v>
+        <v>62</v>
+      </c>
+      <c r="P9" t="s">
+        <v>60</v>
       </c>
       <c r="Q9" t="s">
         <v>52</v>
@@ -1268,13 +1244,13 @@
         <v>56</v>
       </c>
       <c r="V9" t="s">
-        <v>68</v>
+        <v>71</v>
       </c>
       <c r="W9" t="s">
         <v>52</v>
       </c>
       <c r="X9" t="s">
-        <v>99</v>
+        <v>102</v>
       </c>
     </row>
     <row r="10" spans="1:24">
@@ -1302,17 +1278,17 @@
       <c r="L10" t="s">
         <v>57</v>
       </c>
-      <c r="M10">
-        <v>3</v>
-      </c>
-      <c r="N10">
-        <v>5</v>
+      <c r="M10" t="s">
+        <v>60</v>
+      </c>
+      <c r="N10" t="s">
+        <v>61</v>
       </c>
       <c r="O10" t="s">
-        <v>59</v>
-      </c>
-      <c r="P10">
-        <v>2</v>
+        <v>62</v>
+      </c>
+      <c r="P10" t="s">
+        <v>60</v>
       </c>
       <c r="Q10" t="s">
         <v>52</v>
@@ -1330,13 +1306,13 @@
         <v>56</v>
       </c>
       <c r="V10" t="s">
-        <v>68</v>
+        <v>71</v>
       </c>
       <c r="W10" t="s">
         <v>52</v>
       </c>
       <c r="X10" t="s">
-        <v>99</v>
+        <v>102</v>
       </c>
     </row>
     <row r="11" spans="1:24">
@@ -1361,17 +1337,17 @@
       <c r="K11" t="s">
         <v>51</v>
       </c>
-      <c r="M11">
-        <v>5</v>
-      </c>
-      <c r="N11">
-        <v>5</v>
+      <c r="M11" t="s">
+        <v>61</v>
+      </c>
+      <c r="N11" t="s">
+        <v>61</v>
       </c>
       <c r="O11" t="s">
-        <v>62</v>
-      </c>
-      <c r="P11">
-        <v>2</v>
+        <v>65</v>
+      </c>
+      <c r="P11" t="s">
+        <v>60</v>
       </c>
       <c r="Q11" t="s">
         <v>56</v>
@@ -1395,7 +1371,7 @@
         <v>52</v>
       </c>
       <c r="X11" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
     </row>
     <row r="12" spans="1:24">
@@ -1420,17 +1396,17 @@
       <c r="K12" t="s">
         <v>51</v>
       </c>
-      <c r="M12">
-        <v>1</v>
-      </c>
-      <c r="N12">
-        <v>2</v>
+      <c r="M12" t="s">
+        <v>59</v>
+      </c>
+      <c r="N12" t="s">
+        <v>60</v>
       </c>
       <c r="O12" t="s">
+        <v>62</v>
+      </c>
+      <c r="P12" t="s">
         <v>59</v>
-      </c>
-      <c r="P12">
-        <v>1</v>
       </c>
       <c r="Q12" t="s">
         <v>52</v>
@@ -1449,6 +1425,9 @@
       </c>
       <c r="W12" t="s">
         <v>56</v>
+      </c>
+      <c r="X12" t="s">
+        <v>100</v>
       </c>
     </row>
     <row r="13" spans="1:24">
@@ -1473,17 +1452,17 @@
       <c r="K13" t="s">
         <v>51</v>
       </c>
-      <c r="M13">
-        <v>3</v>
-      </c>
-      <c r="N13">
-        <v>3</v>
+      <c r="M13" t="s">
+        <v>60</v>
+      </c>
+      <c r="N13" t="s">
+        <v>60</v>
       </c>
       <c r="O13" t="s">
+        <v>62</v>
+      </c>
+      <c r="P13" t="s">
         <v>59</v>
-      </c>
-      <c r="P13">
-        <v>0</v>
       </c>
       <c r="Q13" t="s">
         <v>56</v>
@@ -1502,6 +1481,9 @@
       </c>
       <c r="W13" t="s">
         <v>56</v>
+      </c>
+      <c r="X13" t="s">
+        <v>100</v>
       </c>
     </row>
     <row r="14" spans="1:24">
@@ -1523,17 +1505,17 @@
       <c r="K14" t="s">
         <v>51</v>
       </c>
-      <c r="M14">
-        <v>5</v>
-      </c>
-      <c r="N14">
-        <v>5</v>
+      <c r="M14" t="s">
+        <v>61</v>
+      </c>
+      <c r="N14" t="s">
+        <v>61</v>
       </c>
       <c r="O14" t="s">
+        <v>62</v>
+      </c>
+      <c r="P14" t="s">
         <v>59</v>
-      </c>
-      <c r="P14">
-        <v>1</v>
       </c>
       <c r="Q14" t="s">
         <v>56</v>
@@ -1551,10 +1533,13 @@
         <v>52</v>
       </c>
       <c r="V14" t="s">
-        <v>69</v>
+        <v>72</v>
       </c>
       <c r="W14" t="s">
         <v>56</v>
+      </c>
+      <c r="X14" t="s">
+        <v>100</v>
       </c>
     </row>
     <row r="15" spans="1:24">
@@ -1576,17 +1561,17 @@
       <c r="K15" t="s">
         <v>51</v>
       </c>
-      <c r="M15">
-        <v>2</v>
-      </c>
-      <c r="N15">
-        <v>3</v>
+      <c r="M15" t="s">
+        <v>60</v>
+      </c>
+      <c r="N15" t="s">
+        <v>60</v>
       </c>
       <c r="O15" t="s">
-        <v>62</v>
-      </c>
-      <c r="P15">
-        <v>2</v>
+        <v>65</v>
+      </c>
+      <c r="P15" t="s">
+        <v>60</v>
       </c>
       <c r="Q15" t="s">
         <v>56</v>
@@ -1604,10 +1589,13 @@
         <v>56</v>
       </c>
       <c r="V15" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="W15" t="s">
         <v>52</v>
+      </c>
+      <c r="X15" t="s">
+        <v>100</v>
       </c>
     </row>
     <row r="16" spans="1:24">
@@ -1635,17 +1623,17 @@
       <c r="L16" t="s">
         <v>57</v>
       </c>
-      <c r="M16">
-        <v>3</v>
-      </c>
-      <c r="N16">
-        <v>3</v>
+      <c r="M16" t="s">
+        <v>60</v>
+      </c>
+      <c r="N16" t="s">
+        <v>60</v>
       </c>
       <c r="O16" t="s">
-        <v>59</v>
-      </c>
-      <c r="P16">
-        <v>2</v>
+        <v>62</v>
+      </c>
+      <c r="P16" t="s">
+        <v>60</v>
       </c>
       <c r="Q16" t="s">
         <v>56</v>
@@ -1663,13 +1651,13 @@
         <v>56</v>
       </c>
       <c r="V16" t="s">
-        <v>70</v>
+        <v>73</v>
       </c>
       <c r="W16" t="s">
         <v>52</v>
       </c>
       <c r="X16" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
     </row>
     <row r="17" spans="1:24">
@@ -1691,17 +1679,17 @@
       <c r="K17" t="s">
         <v>51</v>
       </c>
-      <c r="M17">
-        <v>1</v>
-      </c>
-      <c r="N17">
-        <v>5</v>
+      <c r="M17" t="s">
+        <v>59</v>
+      </c>
+      <c r="N17" t="s">
+        <v>61</v>
       </c>
       <c r="O17" t="s">
-        <v>59</v>
-      </c>
-      <c r="P17">
-        <v>5</v>
+        <v>62</v>
+      </c>
+      <c r="P17" t="s">
+        <v>61</v>
       </c>
       <c r="Q17" t="s">
         <v>52</v>
@@ -1719,13 +1707,13 @@
         <v>56</v>
       </c>
       <c r="V17" t="s">
-        <v>71</v>
+        <v>74</v>
       </c>
       <c r="W17" t="s">
         <v>52</v>
       </c>
       <c r="X17" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="18" spans="1:24">
@@ -1759,17 +1747,17 @@
       <c r="K18" t="s">
         <v>51</v>
       </c>
-      <c r="M18">
-        <v>5</v>
-      </c>
-      <c r="N18">
-        <v>5</v>
+      <c r="M18" t="s">
+        <v>61</v>
+      </c>
+      <c r="N18" t="s">
+        <v>61</v>
       </c>
       <c r="O18" t="s">
-        <v>59</v>
-      </c>
-      <c r="P18">
-        <v>2</v>
+        <v>62</v>
+      </c>
+      <c r="P18" t="s">
+        <v>60</v>
       </c>
       <c r="Q18" t="s">
         <v>52</v>
@@ -1787,10 +1775,13 @@
         <v>52</v>
       </c>
       <c r="V18" t="s">
-        <v>72</v>
+        <v>75</v>
       </c>
       <c r="W18" t="s">
         <v>52</v>
+      </c>
+      <c r="X18" t="s">
+        <v>100</v>
       </c>
     </row>
     <row r="19" spans="1:24">
@@ -1815,17 +1806,17 @@
       <c r="K19" t="s">
         <v>51</v>
       </c>
-      <c r="M19">
-        <v>4</v>
-      </c>
-      <c r="N19">
-        <v>5</v>
+      <c r="M19" t="s">
+        <v>61</v>
+      </c>
+      <c r="N19" t="s">
+        <v>61</v>
       </c>
       <c r="O19" t="s">
+        <v>62</v>
+      </c>
+      <c r="P19" t="s">
         <v>59</v>
-      </c>
-      <c r="P19">
-        <v>0</v>
       </c>
       <c r="Q19" t="s">
         <v>56</v>
@@ -1843,13 +1834,13 @@
         <v>52</v>
       </c>
       <c r="V19" t="s">
-        <v>73</v>
+        <v>76</v>
       </c>
       <c r="W19" t="s">
         <v>52</v>
       </c>
       <c r="X19" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="20" spans="1:24">
@@ -1874,17 +1865,17 @@
       <c r="K20" t="s">
         <v>51</v>
       </c>
-      <c r="M20">
-        <v>5</v>
-      </c>
-      <c r="N20">
-        <v>5</v>
+      <c r="M20" t="s">
+        <v>61</v>
+      </c>
+      <c r="N20" t="s">
+        <v>61</v>
       </c>
       <c r="O20" t="s">
+        <v>62</v>
+      </c>
+      <c r="P20" t="s">
         <v>59</v>
-      </c>
-      <c r="P20">
-        <v>1</v>
       </c>
       <c r="Q20" t="s">
         <v>56</v>
@@ -1905,7 +1896,7 @@
         <v>52</v>
       </c>
       <c r="X20" t="s">
-        <v>97</v>
+        <v>101</v>
       </c>
     </row>
     <row r="21" spans="1:24">
@@ -1930,17 +1921,17 @@
       <c r="K21" t="s">
         <v>51</v>
       </c>
-      <c r="M21">
-        <v>5</v>
-      </c>
-      <c r="N21">
-        <v>3</v>
+      <c r="M21" t="s">
+        <v>61</v>
+      </c>
+      <c r="N21" t="s">
+        <v>60</v>
       </c>
       <c r="O21" t="s">
-        <v>59</v>
-      </c>
-      <c r="P21">
-        <v>3</v>
+        <v>62</v>
+      </c>
+      <c r="P21" t="s">
+        <v>60</v>
       </c>
       <c r="Q21" t="s">
         <v>56</v>
@@ -1959,6 +1950,9 @@
       </c>
       <c r="W21" t="s">
         <v>52</v>
+      </c>
+      <c r="X21" t="s">
+        <v>100</v>
       </c>
     </row>
     <row r="22" spans="1:24">
@@ -1989,17 +1983,17 @@
       <c r="L22" t="s">
         <v>58</v>
       </c>
-      <c r="M22">
-        <v>3</v>
-      </c>
-      <c r="N22">
-        <v>4</v>
+      <c r="M22" t="s">
+        <v>60</v>
+      </c>
+      <c r="N22" t="s">
+        <v>61</v>
       </c>
       <c r="O22" t="s">
-        <v>59</v>
-      </c>
-      <c r="P22">
-        <v>4</v>
+        <v>62</v>
+      </c>
+      <c r="P22" t="s">
+        <v>61</v>
       </c>
       <c r="Q22" t="s">
         <v>52</v>
@@ -2023,7 +2017,7 @@
         <v>52</v>
       </c>
       <c r="X22" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="23" spans="1:24">
@@ -2048,17 +2042,17 @@
       <c r="K23" t="s">
         <v>51</v>
       </c>
-      <c r="M23">
-        <v>5</v>
-      </c>
-      <c r="N23">
-        <v>3</v>
+      <c r="M23" t="s">
+        <v>61</v>
+      </c>
+      <c r="N23" t="s">
+        <v>60</v>
       </c>
       <c r="O23" t="s">
+        <v>62</v>
+      </c>
+      <c r="P23" t="s">
         <v>59</v>
-      </c>
-      <c r="P23">
-        <v>0</v>
       </c>
       <c r="Q23" t="s">
         <v>56</v>
@@ -2077,6 +2071,9 @@
       </c>
       <c r="W23" t="s">
         <v>56</v>
+      </c>
+      <c r="X23" t="s">
+        <v>100</v>
       </c>
     </row>
     <row r="24" spans="1:24">
@@ -2098,17 +2095,17 @@
       <c r="K24" t="s">
         <v>51</v>
       </c>
-      <c r="M24">
-        <v>3</v>
-      </c>
-      <c r="N24">
-        <v>5</v>
+      <c r="M24" t="s">
+        <v>60</v>
+      </c>
+      <c r="N24" t="s">
+        <v>61</v>
       </c>
       <c r="O24" t="s">
-        <v>59</v>
-      </c>
-      <c r="P24">
-        <v>3</v>
+        <v>62</v>
+      </c>
+      <c r="P24" t="s">
+        <v>60</v>
       </c>
       <c r="Q24" t="s">
         <v>56</v>
@@ -2126,13 +2123,13 @@
         <v>52</v>
       </c>
       <c r="V24" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
       <c r="W24" t="s">
         <v>52</v>
       </c>
       <c r="X24" t="s">
-        <v>105</v>
+        <v>99</v>
       </c>
     </row>
     <row r="25" spans="1:24">
@@ -2160,17 +2157,17 @@
       <c r="K25" t="s">
         <v>51</v>
       </c>
-      <c r="M25">
-        <v>5</v>
-      </c>
-      <c r="N25">
-        <v>3</v>
+      <c r="M25" t="s">
+        <v>61</v>
+      </c>
+      <c r="N25" t="s">
+        <v>60</v>
       </c>
       <c r="O25" t="s">
-        <v>59</v>
-      </c>
-      <c r="P25">
-        <v>5</v>
+        <v>62</v>
+      </c>
+      <c r="P25" t="s">
+        <v>61</v>
       </c>
       <c r="Q25" t="s">
         <v>52</v>
@@ -2189,6 +2186,9 @@
       </c>
       <c r="W25" t="s">
         <v>56</v>
+      </c>
+      <c r="X25" t="s">
+        <v>100</v>
       </c>
     </row>
     <row r="26" spans="1:24">
@@ -2213,17 +2213,17 @@
       <c r="K26" t="s">
         <v>51</v>
       </c>
-      <c r="M26">
-        <v>5</v>
-      </c>
-      <c r="N26">
-        <v>5</v>
+      <c r="M26" t="s">
+        <v>61</v>
+      </c>
+      <c r="N26" t="s">
+        <v>61</v>
       </c>
       <c r="O26" t="s">
+        <v>62</v>
+      </c>
+      <c r="P26" t="s">
         <v>59</v>
-      </c>
-      <c r="P26">
-        <v>0</v>
       </c>
       <c r="Q26" t="s">
         <v>56</v>
@@ -2241,10 +2241,13 @@
         <v>56</v>
       </c>
       <c r="V26" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
       <c r="W26" t="s">
         <v>56</v>
+      </c>
+      <c r="X26" t="s">
+        <v>100</v>
       </c>
     </row>
     <row r="27" spans="1:24">
@@ -2266,17 +2269,17 @@
       <c r="K27" t="s">
         <v>51</v>
       </c>
-      <c r="M27">
-        <v>5</v>
-      </c>
-      <c r="N27">
-        <v>5</v>
+      <c r="M27" t="s">
+        <v>61</v>
+      </c>
+      <c r="N27" t="s">
+        <v>61</v>
       </c>
       <c r="O27" t="s">
+        <v>62</v>
+      </c>
+      <c r="P27" t="s">
         <v>59</v>
-      </c>
-      <c r="P27">
-        <v>0</v>
       </c>
       <c r="Q27" t="s">
         <v>56</v>
@@ -2294,10 +2297,13 @@
         <v>52</v>
       </c>
       <c r="V27" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
       <c r="W27" t="s">
         <v>56</v>
+      </c>
+      <c r="X27" t="s">
+        <v>100</v>
       </c>
     </row>
     <row r="28" spans="1:24">
@@ -2328,17 +2334,17 @@
       <c r="L28" t="s">
         <v>58</v>
       </c>
-      <c r="M28">
-        <v>4</v>
-      </c>
-      <c r="N28">
-        <v>3</v>
+      <c r="M28" t="s">
+        <v>61</v>
+      </c>
+      <c r="N28" t="s">
+        <v>60</v>
       </c>
       <c r="O28" t="s">
-        <v>61</v>
-      </c>
-      <c r="P28">
-        <v>2</v>
+        <v>64</v>
+      </c>
+      <c r="P28" t="s">
+        <v>60</v>
       </c>
       <c r="Q28" t="s">
         <v>52</v>
@@ -2359,7 +2365,7 @@
         <v>52</v>
       </c>
       <c r="X28" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
     </row>
     <row r="29" spans="1:24">
@@ -2390,17 +2396,17 @@
       <c r="K29" t="s">
         <v>51</v>
       </c>
-      <c r="M29">
-        <v>3</v>
-      </c>
-      <c r="N29">
-        <v>1</v>
+      <c r="M29" t="s">
+        <v>60</v>
+      </c>
+      <c r="N29" t="s">
+        <v>59</v>
       </c>
       <c r="O29" t="s">
+        <v>62</v>
+      </c>
+      <c r="P29" t="s">
         <v>59</v>
-      </c>
-      <c r="P29">
-        <v>1</v>
       </c>
       <c r="Q29" t="s">
         <v>56</v>
@@ -2418,13 +2424,13 @@
         <v>56</v>
       </c>
       <c r="V29" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="W29" t="s">
         <v>52</v>
       </c>
       <c r="X29" t="s">
-        <v>107</v>
+        <v>102</v>
       </c>
     </row>
     <row r="30" spans="1:24">
@@ -2449,17 +2455,17 @@
       <c r="K30" t="s">
         <v>51</v>
       </c>
-      <c r="M30">
-        <v>3</v>
-      </c>
-      <c r="N30">
-        <v>5</v>
+      <c r="M30" t="s">
+        <v>60</v>
+      </c>
+      <c r="N30" t="s">
+        <v>61</v>
       </c>
       <c r="O30" t="s">
-        <v>59</v>
-      </c>
-      <c r="P30">
-        <v>5</v>
+        <v>62</v>
+      </c>
+      <c r="P30" t="s">
+        <v>61</v>
       </c>
       <c r="Q30" t="s">
         <v>56</v>
@@ -2477,13 +2483,13 @@
         <v>56</v>
       </c>
       <c r="V30" t="s">
-        <v>74</v>
+        <v>77</v>
       </c>
       <c r="W30" t="s">
         <v>52</v>
       </c>
       <c r="X30" t="s">
-        <v>108</v>
+        <v>101</v>
       </c>
     </row>
     <row r="31" spans="1:24">
@@ -2508,17 +2514,17 @@
       <c r="K31" t="s">
         <v>51</v>
       </c>
-      <c r="M31">
-        <v>3</v>
-      </c>
-      <c r="N31">
-        <v>2</v>
+      <c r="M31" t="s">
+        <v>60</v>
+      </c>
+      <c r="N31" t="s">
+        <v>60</v>
       </c>
       <c r="O31" t="s">
-        <v>59</v>
-      </c>
-      <c r="P31">
-        <v>4</v>
+        <v>62</v>
+      </c>
+      <c r="P31" t="s">
+        <v>61</v>
       </c>
       <c r="Q31" t="s">
         <v>56</v>
@@ -2536,13 +2542,13 @@
         <v>52</v>
       </c>
       <c r="V31" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="W31" t="s">
         <v>52</v>
       </c>
       <c r="X31" t="s">
-        <v>109</v>
+        <v>101</v>
       </c>
     </row>
     <row r="32" spans="1:24">
@@ -2579,17 +2585,17 @@
       <c r="K32" t="s">
         <v>51</v>
       </c>
-      <c r="M32">
-        <v>5</v>
-      </c>
-      <c r="N32">
-        <v>5</v>
+      <c r="M32" t="s">
+        <v>61</v>
+      </c>
+      <c r="N32" t="s">
+        <v>61</v>
       </c>
       <c r="O32" t="s">
+        <v>62</v>
+      </c>
+      <c r="P32" t="s">
         <v>59</v>
-      </c>
-      <c r="P32">
-        <v>0</v>
       </c>
       <c r="Q32" t="s">
         <v>56</v>
@@ -2607,13 +2613,13 @@
         <v>56</v>
       </c>
       <c r="V32" t="s">
-        <v>72</v>
+        <v>75</v>
       </c>
       <c r="W32" t="s">
         <v>52</v>
       </c>
       <c r="X32" t="s">
-        <v>109</v>
+        <v>101</v>
       </c>
     </row>
     <row r="33" spans="1:24">
@@ -2650,17 +2656,17 @@
       <c r="K33" t="s">
         <v>52</v>
       </c>
-      <c r="M33">
-        <v>2</v>
-      </c>
-      <c r="N33">
-        <v>2</v>
+      <c r="M33" t="s">
+        <v>60</v>
+      </c>
+      <c r="N33" t="s">
+        <v>60</v>
       </c>
       <c r="O33" t="s">
-        <v>59</v>
-      </c>
-      <c r="P33">
-        <v>3</v>
+        <v>62</v>
+      </c>
+      <c r="P33" t="s">
+        <v>60</v>
       </c>
       <c r="Q33" t="s">
         <v>56</v>
@@ -2678,13 +2684,13 @@
         <v>56</v>
       </c>
       <c r="V33" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="W33" t="s">
         <v>52</v>
       </c>
       <c r="X33" t="s">
-        <v>110</v>
+        <v>102</v>
       </c>
     </row>
     <row r="34" spans="1:24">
@@ -2709,17 +2715,17 @@
       <c r="K34" t="s">
         <v>51</v>
       </c>
-      <c r="M34">
-        <v>3</v>
-      </c>
-      <c r="N34">
-        <v>2</v>
+      <c r="M34" t="s">
+        <v>60</v>
+      </c>
+      <c r="N34" t="s">
+        <v>60</v>
       </c>
       <c r="O34" t="s">
+        <v>62</v>
+      </c>
+      <c r="P34" t="s">
         <v>59</v>
-      </c>
-      <c r="P34">
-        <v>0</v>
       </c>
       <c r="Q34" t="s">
         <v>56</v>
@@ -2738,6 +2744,9 @@
       </c>
       <c r="W34" t="s">
         <v>56</v>
+      </c>
+      <c r="X34" t="s">
+        <v>100</v>
       </c>
     </row>
     <row r="35" spans="1:24">
@@ -2765,17 +2774,17 @@
       <c r="K35" t="s">
         <v>51</v>
       </c>
-      <c r="M35">
-        <v>5</v>
-      </c>
-      <c r="N35">
-        <v>5</v>
+      <c r="M35" t="s">
+        <v>61</v>
+      </c>
+      <c r="N35" t="s">
+        <v>61</v>
       </c>
       <c r="O35" t="s">
-        <v>61</v>
-      </c>
-      <c r="P35">
-        <v>2</v>
+        <v>64</v>
+      </c>
+      <c r="P35" t="s">
+        <v>60</v>
       </c>
       <c r="Q35" t="s">
         <v>56</v>
@@ -2796,7 +2805,7 @@
         <v>52</v>
       </c>
       <c r="X35" t="s">
-        <v>109</v>
+        <v>101</v>
       </c>
     </row>
     <row r="36" spans="1:24">
@@ -2821,17 +2830,17 @@
       <c r="K36" t="s">
         <v>51</v>
       </c>
-      <c r="M36">
-        <v>5</v>
-      </c>
-      <c r="N36">
-        <v>2</v>
+      <c r="M36" t="s">
+        <v>61</v>
+      </c>
+      <c r="N36" t="s">
+        <v>60</v>
       </c>
       <c r="O36" t="s">
-        <v>59</v>
-      </c>
-      <c r="P36">
-        <v>2</v>
+        <v>62</v>
+      </c>
+      <c r="P36" t="s">
+        <v>60</v>
       </c>
       <c r="Q36" t="s">
         <v>56</v>
@@ -2849,13 +2858,13 @@
         <v>52</v>
       </c>
       <c r="V36" t="s">
-        <v>77</v>
+        <v>80</v>
       </c>
       <c r="W36" t="s">
         <v>52</v>
       </c>
       <c r="X36" t="s">
-        <v>109</v>
+        <v>101</v>
       </c>
     </row>
     <row r="37" spans="1:24">
@@ -2880,17 +2889,17 @@
       <c r="K37" t="s">
         <v>51</v>
       </c>
-      <c r="M37">
-        <v>3</v>
-      </c>
-      <c r="N37">
-        <v>5</v>
+      <c r="M37" t="s">
+        <v>60</v>
+      </c>
+      <c r="N37" t="s">
+        <v>61</v>
       </c>
       <c r="O37" t="s">
-        <v>59</v>
-      </c>
-      <c r="P37">
-        <v>3</v>
+        <v>62</v>
+      </c>
+      <c r="P37" t="s">
+        <v>60</v>
       </c>
       <c r="Q37" t="s">
         <v>56</v>
@@ -2908,13 +2917,13 @@
         <v>56</v>
       </c>
       <c r="V37" t="s">
-        <v>78</v>
+        <v>81</v>
       </c>
       <c r="W37" t="s">
         <v>52</v>
       </c>
       <c r="X37" t="s">
-        <v>109</v>
+        <v>101</v>
       </c>
     </row>
     <row r="38" spans="1:24">
@@ -2942,17 +2951,17 @@
       <c r="K38" t="s">
         <v>51</v>
       </c>
-      <c r="M38">
-        <v>5</v>
-      </c>
-      <c r="N38">
-        <v>5</v>
+      <c r="M38" t="s">
+        <v>61</v>
+      </c>
+      <c r="N38" t="s">
+        <v>61</v>
       </c>
       <c r="O38" t="s">
+        <v>62</v>
+      </c>
+      <c r="P38" t="s">
         <v>59</v>
-      </c>
-      <c r="P38">
-        <v>0</v>
       </c>
       <c r="Q38" t="s">
         <v>56</v>
@@ -2970,13 +2979,13 @@
         <v>56</v>
       </c>
       <c r="V38" t="s">
-        <v>68</v>
+        <v>71</v>
       </c>
       <c r="W38" t="s">
         <v>52</v>
       </c>
       <c r="X38" t="s">
-        <v>109</v>
+        <v>101</v>
       </c>
     </row>
     <row r="39" spans="1:24">
@@ -3004,17 +3013,17 @@
       <c r="K39" t="s">
         <v>51</v>
       </c>
-      <c r="M39">
-        <v>3</v>
-      </c>
-      <c r="N39">
-        <v>4</v>
+      <c r="M39" t="s">
+        <v>60</v>
+      </c>
+      <c r="N39" t="s">
+        <v>61</v>
       </c>
       <c r="O39" t="s">
-        <v>61</v>
-      </c>
-      <c r="P39">
-        <v>1</v>
+        <v>64</v>
+      </c>
+      <c r="P39" t="s">
+        <v>59</v>
       </c>
       <c r="Q39" t="s">
         <v>56</v>
@@ -3032,10 +3041,13 @@
         <v>56</v>
       </c>
       <c r="V39" t="s">
-        <v>79</v>
+        <v>82</v>
       </c>
       <c r="W39" t="s">
         <v>56</v>
+      </c>
+      <c r="X39" t="s">
+        <v>100</v>
       </c>
     </row>
     <row r="40" spans="1:24">
@@ -3063,17 +3075,17 @@
       <c r="K40" t="s">
         <v>51</v>
       </c>
-      <c r="M40">
-        <v>5</v>
-      </c>
-      <c r="N40">
-        <v>5</v>
+      <c r="M40" t="s">
+        <v>61</v>
+      </c>
+      <c r="N40" t="s">
+        <v>61</v>
       </c>
       <c r="O40" t="s">
         <v>54</v>
       </c>
-      <c r="P40">
-        <v>4</v>
+      <c r="P40" t="s">
+        <v>61</v>
       </c>
       <c r="Q40" t="s">
         <v>52</v>
@@ -3097,7 +3109,7 @@
         <v>52</v>
       </c>
       <c r="X40" t="s">
-        <v>109</v>
+        <v>101</v>
       </c>
     </row>
     <row r="41" spans="1:24">
@@ -3131,17 +3143,17 @@
       <c r="K41" t="s">
         <v>51</v>
       </c>
-      <c r="M41">
-        <v>4</v>
-      </c>
-      <c r="N41">
-        <v>5</v>
+      <c r="M41" t="s">
+        <v>61</v>
+      </c>
+      <c r="N41" t="s">
+        <v>61</v>
       </c>
       <c r="O41" t="s">
         <v>54</v>
       </c>
-      <c r="P41">
-        <v>5</v>
+      <c r="P41" t="s">
+        <v>61</v>
       </c>
       <c r="Q41" t="s">
         <v>56</v>
@@ -3162,7 +3174,7 @@
         <v>52</v>
       </c>
       <c r="X41" t="s">
-        <v>109</v>
+        <v>101</v>
       </c>
     </row>
     <row r="42" spans="1:24">
@@ -3190,17 +3202,17 @@
       <c r="K42" t="s">
         <v>51</v>
       </c>
-      <c r="M42">
-        <v>2</v>
-      </c>
-      <c r="N42">
-        <v>5</v>
+      <c r="M42" t="s">
+        <v>60</v>
+      </c>
+      <c r="N42" t="s">
+        <v>61</v>
       </c>
       <c r="O42" t="s">
+        <v>62</v>
+      </c>
+      <c r="P42" t="s">
         <v>59</v>
-      </c>
-      <c r="P42">
-        <v>0</v>
       </c>
       <c r="Q42" t="s">
         <v>56</v>
@@ -3218,13 +3230,13 @@
         <v>56</v>
       </c>
       <c r="V42" t="s">
-        <v>80</v>
+        <v>83</v>
       </c>
       <c r="W42" t="s">
         <v>52</v>
       </c>
       <c r="X42" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
     </row>
     <row r="43" spans="1:24">
@@ -3249,17 +3261,17 @@
       <c r="K43" t="s">
         <v>51</v>
       </c>
-      <c r="M43">
-        <v>4</v>
-      </c>
-      <c r="N43">
-        <v>5</v>
+      <c r="M43" t="s">
+        <v>61</v>
+      </c>
+      <c r="N43" t="s">
+        <v>61</v>
       </c>
       <c r="O43" t="s">
-        <v>59</v>
-      </c>
-      <c r="P43">
-        <v>2</v>
+        <v>62</v>
+      </c>
+      <c r="P43" t="s">
+        <v>60</v>
       </c>
       <c r="Q43" t="s">
         <v>52</v>
@@ -3283,7 +3295,7 @@
         <v>52</v>
       </c>
       <c r="X43" t="s">
-        <v>111</v>
+        <v>99</v>
       </c>
     </row>
     <row r="44" spans="1:24">
@@ -3311,17 +3323,17 @@
       <c r="K44" t="s">
         <v>51</v>
       </c>
-      <c r="M44">
-        <v>4</v>
-      </c>
-      <c r="N44">
-        <v>3</v>
+      <c r="M44" t="s">
+        <v>61</v>
+      </c>
+      <c r="N44" t="s">
+        <v>60</v>
       </c>
       <c r="O44" t="s">
+        <v>62</v>
+      </c>
+      <c r="P44" t="s">
         <v>59</v>
-      </c>
-      <c r="P44">
-        <v>1</v>
       </c>
       <c r="Q44" t="s">
         <v>56</v>
@@ -3339,13 +3351,13 @@
         <v>56</v>
       </c>
       <c r="V44" t="s">
-        <v>81</v>
+        <v>84</v>
       </c>
       <c r="W44" t="s">
         <v>52</v>
       </c>
       <c r="X44" t="s">
-        <v>109</v>
+        <v>101</v>
       </c>
     </row>
     <row r="45" spans="1:24">
@@ -3370,17 +3382,17 @@
       <c r="K45" t="s">
         <v>51</v>
       </c>
-      <c r="M45">
-        <v>4</v>
-      </c>
-      <c r="N45">
-        <v>5</v>
+      <c r="M45" t="s">
+        <v>61</v>
+      </c>
+      <c r="N45" t="s">
+        <v>61</v>
       </c>
       <c r="O45" t="s">
+        <v>62</v>
+      </c>
+      <c r="P45" t="s">
         <v>59</v>
-      </c>
-      <c r="P45">
-        <v>0</v>
       </c>
       <c r="Q45" t="s">
         <v>56</v>
@@ -3404,7 +3416,7 @@
         <v>52</v>
       </c>
       <c r="X45" t="s">
-        <v>112</v>
+        <v>102</v>
       </c>
     </row>
     <row r="46" spans="1:24">
@@ -3441,17 +3453,17 @@
       <c r="L46" t="s">
         <v>58</v>
       </c>
-      <c r="M46">
-        <v>1</v>
-      </c>
-      <c r="N46">
-        <v>4</v>
+      <c r="M46" t="s">
+        <v>59</v>
+      </c>
+      <c r="N46" t="s">
+        <v>61</v>
       </c>
       <c r="O46" t="s">
-        <v>61</v>
-      </c>
-      <c r="P46">
-        <v>3</v>
+        <v>64</v>
+      </c>
+      <c r="P46" t="s">
+        <v>60</v>
       </c>
       <c r="Q46" t="s">
         <v>56</v>
@@ -3472,7 +3484,7 @@
         <v>56</v>
       </c>
       <c r="X46" t="s">
-        <v>109</v>
+        <v>101</v>
       </c>
     </row>
     <row r="47" spans="1:24">
@@ -3497,17 +3509,17 @@
       <c r="K47" t="s">
         <v>51</v>
       </c>
-      <c r="M47">
-        <v>3</v>
-      </c>
-      <c r="N47">
-        <v>3</v>
+      <c r="M47" t="s">
+        <v>60</v>
+      </c>
+      <c r="N47" t="s">
+        <v>60</v>
       </c>
       <c r="O47" t="s">
+        <v>62</v>
+      </c>
+      <c r="P47" t="s">
         <v>59</v>
-      </c>
-      <c r="P47">
-        <v>1</v>
       </c>
       <c r="Q47" t="s">
         <v>56</v>
@@ -3528,7 +3540,7 @@
         <v>52</v>
       </c>
       <c r="X47" t="s">
-        <v>109</v>
+        <v>101</v>
       </c>
     </row>
     <row r="48" spans="1:24">
@@ -3553,17 +3565,17 @@
       <c r="K48" t="s">
         <v>51</v>
       </c>
-      <c r="M48">
-        <v>4</v>
-      </c>
-      <c r="N48">
-        <v>2</v>
+      <c r="M48" t="s">
+        <v>61</v>
+      </c>
+      <c r="N48" t="s">
+        <v>60</v>
       </c>
       <c r="O48" t="s">
+        <v>62</v>
+      </c>
+      <c r="P48" t="s">
         <v>59</v>
-      </c>
-      <c r="P48">
-        <v>0</v>
       </c>
       <c r="Q48" t="s">
         <v>52</v>
@@ -3581,10 +3593,13 @@
         <v>52</v>
       </c>
       <c r="V48" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
       <c r="W48" t="s">
         <v>56</v>
+      </c>
+      <c r="X48" t="s">
+        <v>100</v>
       </c>
     </row>
     <row r="49" spans="1:24">
@@ -3621,17 +3636,17 @@
       <c r="L49" t="s">
         <v>58</v>
       </c>
-      <c r="M49">
-        <v>4</v>
-      </c>
-      <c r="N49">
-        <v>5</v>
+      <c r="M49" t="s">
+        <v>61</v>
+      </c>
+      <c r="N49" t="s">
+        <v>61</v>
       </c>
       <c r="O49" t="s">
         <v>54</v>
       </c>
-      <c r="P49">
-        <v>0</v>
+      <c r="P49" t="s">
+        <v>59</v>
       </c>
       <c r="Q49" t="s">
         <v>56</v>
@@ -3649,13 +3664,13 @@
         <v>56</v>
       </c>
       <c r="V49" t="s">
-        <v>82</v>
+        <v>85</v>
       </c>
       <c r="W49" t="s">
         <v>52</v>
       </c>
       <c r="X49" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
     </row>
     <row r="50" spans="1:24">
@@ -3680,17 +3695,17 @@
       <c r="K50" t="s">
         <v>51</v>
       </c>
-      <c r="M50">
-        <v>3</v>
-      </c>
-      <c r="N50">
-        <v>5</v>
+      <c r="M50" t="s">
+        <v>60</v>
+      </c>
+      <c r="N50" t="s">
+        <v>61</v>
       </c>
       <c r="O50" t="s">
+        <v>62</v>
+      </c>
+      <c r="P50" t="s">
         <v>59</v>
-      </c>
-      <c r="P50">
-        <v>1</v>
       </c>
       <c r="Q50" t="s">
         <v>56</v>
@@ -3712,6 +3727,9 @@
       </c>
       <c r="W50" t="s">
         <v>56</v>
+      </c>
+      <c r="X50" t="s">
+        <v>100</v>
       </c>
     </row>
     <row r="51" spans="1:24">
@@ -3748,17 +3766,17 @@
       <c r="L51" t="s">
         <v>58</v>
       </c>
-      <c r="M51">
-        <v>4</v>
-      </c>
-      <c r="N51">
-        <v>5</v>
+      <c r="M51" t="s">
+        <v>61</v>
+      </c>
+      <c r="N51" t="s">
+        <v>61</v>
       </c>
       <c r="O51" t="s">
         <v>54</v>
       </c>
-      <c r="P51">
-        <v>1</v>
+      <c r="P51" t="s">
+        <v>59</v>
       </c>
       <c r="Q51" t="s">
         <v>56</v>
@@ -3776,13 +3794,13 @@
         <v>56</v>
       </c>
       <c r="V51" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="W51" t="s">
         <v>52</v>
       </c>
       <c r="X51" t="s">
-        <v>109</v>
+        <v>101</v>
       </c>
     </row>
     <row r="52" spans="1:24">
@@ -3807,17 +3825,17 @@
       <c r="K52" t="s">
         <v>51</v>
       </c>
-      <c r="M52">
-        <v>5</v>
-      </c>
-      <c r="N52">
-        <v>5</v>
+      <c r="M52" t="s">
+        <v>61</v>
+      </c>
+      <c r="N52" t="s">
+        <v>61</v>
       </c>
       <c r="O52" t="s">
+        <v>62</v>
+      </c>
+      <c r="P52" t="s">
         <v>59</v>
-      </c>
-      <c r="P52">
-        <v>0</v>
       </c>
       <c r="Q52" t="s">
         <v>56</v>
@@ -3835,13 +3853,13 @@
         <v>56</v>
       </c>
       <c r="V52" t="s">
-        <v>74</v>
+        <v>77</v>
       </c>
       <c r="W52" t="s">
         <v>52</v>
       </c>
       <c r="X52" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
     </row>
     <row r="53" spans="1:24">
@@ -3866,17 +3884,17 @@
       <c r="K53" t="s">
         <v>51</v>
       </c>
-      <c r="M53">
-        <v>3</v>
-      </c>
-      <c r="N53">
-        <v>4</v>
+      <c r="M53" t="s">
+        <v>60</v>
+      </c>
+      <c r="N53" t="s">
+        <v>61</v>
       </c>
       <c r="O53" t="s">
-        <v>59</v>
-      </c>
-      <c r="P53">
-        <v>2</v>
+        <v>62</v>
+      </c>
+      <c r="P53" t="s">
+        <v>60</v>
       </c>
       <c r="Q53" t="s">
         <v>56</v>
@@ -3898,6 +3916,9 @@
       </c>
       <c r="W53" t="s">
         <v>56</v>
+      </c>
+      <c r="X53" t="s">
+        <v>100</v>
       </c>
     </row>
     <row r="54" spans="1:24">
@@ -3922,17 +3943,17 @@
       <c r="K54" t="s">
         <v>51</v>
       </c>
-      <c r="M54">
-        <v>3</v>
-      </c>
-      <c r="N54">
-        <v>5</v>
+      <c r="M54" t="s">
+        <v>60</v>
+      </c>
+      <c r="N54" t="s">
+        <v>61</v>
       </c>
       <c r="O54" t="s">
+        <v>62</v>
+      </c>
+      <c r="P54" t="s">
         <v>59</v>
-      </c>
-      <c r="P54">
-        <v>1</v>
       </c>
       <c r="Q54" t="s">
         <v>56</v>
@@ -3950,13 +3971,13 @@
         <v>56</v>
       </c>
       <c r="V54" t="s">
-        <v>84</v>
+        <v>87</v>
       </c>
       <c r="W54" t="s">
         <v>52</v>
       </c>
       <c r="X54" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
     </row>
     <row r="55" spans="1:24">
@@ -3984,17 +4005,17 @@
       <c r="K55" t="s">
         <v>51</v>
       </c>
-      <c r="M55">
-        <v>2</v>
-      </c>
-      <c r="N55">
-        <v>3</v>
+      <c r="M55" t="s">
+        <v>60</v>
+      </c>
+      <c r="N55" t="s">
+        <v>60</v>
       </c>
       <c r="O55" t="s">
+        <v>62</v>
+      </c>
+      <c r="P55" t="s">
         <v>59</v>
-      </c>
-      <c r="P55">
-        <v>0</v>
       </c>
       <c r="Q55" t="s">
         <v>56</v>
@@ -4018,7 +4039,7 @@
         <v>52</v>
       </c>
       <c r="X55" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
     </row>
     <row r="56" spans="1:24">
@@ -4043,17 +4064,17 @@
       <c r="K56" t="s">
         <v>51</v>
       </c>
-      <c r="M56">
-        <v>3</v>
-      </c>
-      <c r="N56">
-        <v>4</v>
+      <c r="M56" t="s">
+        <v>60</v>
+      </c>
+      <c r="N56" t="s">
+        <v>61</v>
       </c>
       <c r="O56" t="s">
+        <v>62</v>
+      </c>
+      <c r="P56" t="s">
         <v>59</v>
-      </c>
-      <c r="P56">
-        <v>0</v>
       </c>
       <c r="Q56" t="s">
         <v>56</v>
@@ -4071,13 +4092,13 @@
         <v>56</v>
       </c>
       <c r="V56" t="s">
-        <v>85</v>
+        <v>88</v>
       </c>
       <c r="W56" t="s">
         <v>52</v>
       </c>
       <c r="X56" t="s">
-        <v>109</v>
+        <v>101</v>
       </c>
     </row>
     <row r="57" spans="1:24">
@@ -4102,17 +4123,17 @@
       <c r="K57" t="s">
         <v>51</v>
       </c>
-      <c r="M57">
-        <v>2</v>
-      </c>
-      <c r="N57">
-        <v>3</v>
+      <c r="M57" t="s">
+        <v>60</v>
+      </c>
+      <c r="N57" t="s">
+        <v>60</v>
       </c>
       <c r="O57" t="s">
+        <v>62</v>
+      </c>
+      <c r="P57" t="s">
         <v>59</v>
-      </c>
-      <c r="P57">
-        <v>0</v>
       </c>
       <c r="Q57" t="s">
         <v>56</v>
@@ -4130,13 +4151,13 @@
         <v>56</v>
       </c>
       <c r="V57" t="s">
-        <v>86</v>
+        <v>89</v>
       </c>
       <c r="W57" t="s">
         <v>52</v>
       </c>
       <c r="X57" t="s">
-        <v>109</v>
+        <v>101</v>
       </c>
     </row>
     <row r="58" spans="1:24">
@@ -4161,17 +4182,17 @@
       <c r="K58" t="s">
         <v>51</v>
       </c>
-      <c r="M58">
-        <v>3</v>
-      </c>
-      <c r="N58">
-        <v>5</v>
+      <c r="M58" t="s">
+        <v>60</v>
+      </c>
+      <c r="N58" t="s">
+        <v>61</v>
       </c>
       <c r="O58" t="s">
+        <v>62</v>
+      </c>
+      <c r="P58" t="s">
         <v>59</v>
-      </c>
-      <c r="P58">
-        <v>0</v>
       </c>
       <c r="Q58" t="s">
         <v>56</v>
@@ -4189,13 +4210,13 @@
         <v>52</v>
       </c>
       <c r="V58" t="s">
-        <v>87</v>
+        <v>90</v>
       </c>
       <c r="W58" t="s">
         <v>52</v>
       </c>
       <c r="X58" t="s">
-        <v>113</v>
+        <v>103</v>
       </c>
     </row>
     <row r="59" spans="1:24">
@@ -4220,17 +4241,17 @@
       <c r="K59" t="s">
         <v>51</v>
       </c>
-      <c r="M59">
-        <v>3</v>
-      </c>
-      <c r="N59">
-        <v>5</v>
+      <c r="M59" t="s">
+        <v>60</v>
+      </c>
+      <c r="N59" t="s">
+        <v>61</v>
       </c>
       <c r="O59" t="s">
-        <v>59</v>
-      </c>
-      <c r="P59">
-        <v>2</v>
+        <v>62</v>
+      </c>
+      <c r="P59" t="s">
+        <v>60</v>
       </c>
       <c r="Q59" t="s">
         <v>56</v>
@@ -4248,10 +4269,13 @@
         <v>56</v>
       </c>
       <c r="V59" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="W59" t="s">
         <v>56</v>
+      </c>
+      <c r="X59" t="s">
+        <v>100</v>
       </c>
     </row>
     <row r="60" spans="1:24">
@@ -4276,17 +4300,17 @@
       <c r="K60" t="s">
         <v>51</v>
       </c>
-      <c r="M60">
-        <v>2</v>
-      </c>
-      <c r="N60">
-        <v>3</v>
+      <c r="M60" t="s">
+        <v>60</v>
+      </c>
+      <c r="N60" t="s">
+        <v>60</v>
       </c>
       <c r="O60" t="s">
+        <v>62</v>
+      </c>
+      <c r="P60" t="s">
         <v>59</v>
-      </c>
-      <c r="P60">
-        <v>0</v>
       </c>
       <c r="Q60" t="s">
         <v>56</v>
@@ -4304,13 +4328,13 @@
         <v>56</v>
       </c>
       <c r="V60" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
       <c r="W60" t="s">
         <v>52</v>
       </c>
       <c r="X60" t="s">
-        <v>114</v>
+        <v>103</v>
       </c>
     </row>
     <row r="61" spans="1:24">
@@ -4338,17 +4362,17 @@
       <c r="K61" t="s">
         <v>51</v>
       </c>
-      <c r="M61">
-        <v>4</v>
-      </c>
-      <c r="N61">
-        <v>4</v>
+      <c r="M61" t="s">
+        <v>61</v>
+      </c>
+      <c r="N61" t="s">
+        <v>61</v>
       </c>
       <c r="O61" t="s">
-        <v>59</v>
-      </c>
-      <c r="P61">
-        <v>3</v>
+        <v>62</v>
+      </c>
+      <c r="P61" t="s">
+        <v>60</v>
       </c>
       <c r="Q61" t="s">
         <v>56</v>
@@ -4367,6 +4391,9 @@
       </c>
       <c r="W61" t="s">
         <v>56</v>
+      </c>
+      <c r="X61" t="s">
+        <v>100</v>
       </c>
     </row>
     <row r="62" spans="1:24">
@@ -4394,17 +4421,17 @@
       <c r="K62" t="s">
         <v>51</v>
       </c>
-      <c r="M62">
-        <v>3</v>
-      </c>
-      <c r="N62">
-        <v>4</v>
+      <c r="M62" t="s">
+        <v>60</v>
+      </c>
+      <c r="N62" t="s">
+        <v>61</v>
       </c>
       <c r="O62" t="s">
+        <v>62</v>
+      </c>
+      <c r="P62" t="s">
         <v>59</v>
-      </c>
-      <c r="P62">
-        <v>1</v>
       </c>
       <c r="Q62" t="s">
         <v>56</v>
@@ -4425,7 +4452,7 @@
         <v>52</v>
       </c>
       <c r="X62" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
     </row>
     <row r="63" spans="1:24">
@@ -4453,17 +4480,17 @@
       <c r="K63" t="s">
         <v>51</v>
       </c>
-      <c r="M63">
-        <v>3</v>
-      </c>
-      <c r="N63">
-        <v>4</v>
+      <c r="M63" t="s">
+        <v>60</v>
+      </c>
+      <c r="N63" t="s">
+        <v>61</v>
       </c>
       <c r="O63" t="s">
-        <v>59</v>
-      </c>
-      <c r="P63">
-        <v>3</v>
+        <v>62</v>
+      </c>
+      <c r="P63" t="s">
+        <v>60</v>
       </c>
       <c r="Q63" t="s">
         <v>56</v>
@@ -4481,13 +4508,13 @@
         <v>56</v>
       </c>
       <c r="V63" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
       <c r="W63" t="s">
         <v>52</v>
       </c>
       <c r="X63" t="s">
-        <v>109</v>
+        <v>101</v>
       </c>
     </row>
     <row r="64" spans="1:24">
@@ -4512,17 +4539,17 @@
       <c r="K64" t="s">
         <v>51</v>
       </c>
-      <c r="M64">
-        <v>5</v>
-      </c>
-      <c r="N64">
-        <v>2</v>
+      <c r="M64" t="s">
+        <v>61</v>
+      </c>
+      <c r="N64" t="s">
+        <v>60</v>
       </c>
       <c r="O64" t="s">
-        <v>59</v>
-      </c>
-      <c r="P64">
-        <v>5</v>
+        <v>62</v>
+      </c>
+      <c r="P64" t="s">
+        <v>61</v>
       </c>
       <c r="Q64" t="s">
         <v>56</v>
@@ -4540,13 +4567,13 @@
         <v>52</v>
       </c>
       <c r="V64" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
       <c r="W64" t="s">
         <v>52</v>
       </c>
       <c r="X64" t="s">
-        <v>109</v>
+        <v>101</v>
       </c>
     </row>
     <row r="65" spans="1:24">
@@ -4571,17 +4598,17 @@
       <c r="K65" t="s">
         <v>51</v>
       </c>
-      <c r="M65">
-        <v>3</v>
-      </c>
-      <c r="N65">
-        <v>3</v>
+      <c r="M65" t="s">
+        <v>60</v>
+      </c>
+      <c r="N65" t="s">
+        <v>60</v>
       </c>
       <c r="O65" t="s">
-        <v>59</v>
-      </c>
-      <c r="P65">
-        <v>2</v>
+        <v>62</v>
+      </c>
+      <c r="P65" t="s">
+        <v>60</v>
       </c>
       <c r="Q65" t="s">
         <v>56</v>
@@ -4605,7 +4632,7 @@
         <v>52</v>
       </c>
       <c r="X65" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
     </row>
     <row r="66" spans="1:24">
@@ -4630,17 +4657,17 @@
       <c r="K66" t="s">
         <v>51</v>
       </c>
-      <c r="M66">
-        <v>2</v>
-      </c>
-      <c r="N66">
-        <v>4</v>
+      <c r="M66" t="s">
+        <v>60</v>
+      </c>
+      <c r="N66" t="s">
+        <v>61</v>
       </c>
       <c r="O66" t="s">
         <v>54</v>
       </c>
-      <c r="P66">
-        <v>2</v>
+      <c r="P66" t="s">
+        <v>60</v>
       </c>
       <c r="Q66" t="s">
         <v>56</v>
@@ -4664,7 +4691,7 @@
         <v>52</v>
       </c>
       <c r="X66" t="s">
-        <v>109</v>
+        <v>101</v>
       </c>
     </row>
     <row r="67" spans="1:24">
@@ -4689,17 +4716,17 @@
       <c r="K67" t="s">
         <v>51</v>
       </c>
-      <c r="M67">
-        <v>5</v>
-      </c>
-      <c r="N67">
-        <v>4</v>
+      <c r="M67" t="s">
+        <v>61</v>
+      </c>
+      <c r="N67" t="s">
+        <v>61</v>
       </c>
       <c r="O67" t="s">
-        <v>59</v>
-      </c>
-      <c r="P67">
-        <v>3</v>
+        <v>62</v>
+      </c>
+      <c r="P67" t="s">
+        <v>60</v>
       </c>
       <c r="Q67" t="s">
         <v>56</v>
@@ -4720,7 +4747,7 @@
         <v>52</v>
       </c>
       <c r="X67" t="s">
-        <v>109</v>
+        <v>101</v>
       </c>
     </row>
     <row r="68" spans="1:24">
@@ -4745,17 +4772,17 @@
       <c r="K68" t="s">
         <v>51</v>
       </c>
-      <c r="M68">
-        <v>4</v>
-      </c>
-      <c r="N68">
-        <v>5</v>
+      <c r="M68" t="s">
+        <v>61</v>
+      </c>
+      <c r="N68" t="s">
+        <v>61</v>
       </c>
       <c r="O68" t="s">
+        <v>62</v>
+      </c>
+      <c r="P68" t="s">
         <v>59</v>
-      </c>
-      <c r="P68">
-        <v>1</v>
       </c>
       <c r="Q68" t="s">
         <v>56</v>
@@ -4776,7 +4803,7 @@
         <v>52</v>
       </c>
       <c r="X68" t="s">
-        <v>109</v>
+        <v>101</v>
       </c>
     </row>
     <row r="69" spans="1:24">
@@ -4801,17 +4828,17 @@
       <c r="K69" t="s">
         <v>51</v>
       </c>
-      <c r="M69">
-        <v>2</v>
-      </c>
-      <c r="N69">
-        <v>3</v>
+      <c r="M69" t="s">
+        <v>60</v>
+      </c>
+      <c r="N69" t="s">
+        <v>60</v>
       </c>
       <c r="O69" t="s">
+        <v>62</v>
+      </c>
+      <c r="P69" t="s">
         <v>59</v>
-      </c>
-      <c r="P69">
-        <v>0</v>
       </c>
       <c r="Q69" t="s">
         <v>56</v>
@@ -4829,13 +4856,13 @@
         <v>56</v>
       </c>
       <c r="V69" t="s">
-        <v>86</v>
+        <v>89</v>
       </c>
       <c r="W69" t="s">
         <v>52</v>
       </c>
       <c r="X69" t="s">
-        <v>109</v>
+        <v>101</v>
       </c>
     </row>
     <row r="70" spans="1:24">
@@ -4866,17 +4893,17 @@
       <c r="L70" t="s">
         <v>58</v>
       </c>
-      <c r="M70">
-        <v>3</v>
-      </c>
-      <c r="N70">
-        <v>5</v>
+      <c r="M70" t="s">
+        <v>60</v>
+      </c>
+      <c r="N70" t="s">
+        <v>61</v>
       </c>
       <c r="O70" t="s">
-        <v>59</v>
-      </c>
-      <c r="P70">
-        <v>2</v>
+        <v>62</v>
+      </c>
+      <c r="P70" t="s">
+        <v>60</v>
       </c>
       <c r="Q70" t="s">
         <v>56</v>
@@ -4894,10 +4921,13 @@
         <v>52</v>
       </c>
       <c r="V70" t="s">
-        <v>89</v>
+        <v>92</v>
       </c>
       <c r="W70" t="s">
         <v>56</v>
+      </c>
+      <c r="X70" t="s">
+        <v>100</v>
       </c>
     </row>
     <row r="71" spans="1:24">
@@ -4925,17 +4955,17 @@
       <c r="K71" t="s">
         <v>51</v>
       </c>
-      <c r="M71">
-        <v>3</v>
-      </c>
-      <c r="N71">
-        <v>4</v>
+      <c r="M71" t="s">
+        <v>60</v>
+      </c>
+      <c r="N71" t="s">
+        <v>61</v>
       </c>
       <c r="O71" t="s">
+        <v>62</v>
+      </c>
+      <c r="P71" t="s">
         <v>59</v>
-      </c>
-      <c r="P71">
-        <v>1</v>
       </c>
       <c r="Q71" t="s">
         <v>56</v>
@@ -4953,13 +4983,13 @@
         <v>56</v>
       </c>
       <c r="V71" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
       <c r="W71" t="s">
         <v>52</v>
       </c>
       <c r="X71" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
     </row>
     <row r="72" spans="1:24">
@@ -4984,17 +5014,17 @@
       <c r="K72" t="s">
         <v>51</v>
       </c>
-      <c r="M72">
-        <v>4</v>
-      </c>
-      <c r="N72">
-        <v>5</v>
+      <c r="M72" t="s">
+        <v>61</v>
+      </c>
+      <c r="N72" t="s">
+        <v>61</v>
       </c>
       <c r="O72" t="s">
-        <v>59</v>
-      </c>
-      <c r="P72">
-        <v>4</v>
+        <v>62</v>
+      </c>
+      <c r="P72" t="s">
+        <v>61</v>
       </c>
       <c r="Q72" t="s">
         <v>56</v>
@@ -5016,6 +5046,9 @@
       </c>
       <c r="W72" t="s">
         <v>56</v>
+      </c>
+      <c r="X72" t="s">
+        <v>100</v>
       </c>
     </row>
     <row r="73" spans="1:24">
@@ -5040,17 +5073,17 @@
       <c r="K73" t="s">
         <v>51</v>
       </c>
-      <c r="M73">
-        <v>3</v>
-      </c>
-      <c r="N73">
-        <v>3</v>
+      <c r="M73" t="s">
+        <v>60</v>
+      </c>
+      <c r="N73" t="s">
+        <v>60</v>
       </c>
       <c r="O73" t="s">
+        <v>62</v>
+      </c>
+      <c r="P73" t="s">
         <v>59</v>
-      </c>
-      <c r="P73">
-        <v>0</v>
       </c>
       <c r="Q73" t="s">
         <v>56</v>
@@ -5074,7 +5107,7 @@
         <v>52</v>
       </c>
       <c r="X73" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
     </row>
     <row r="74" spans="1:24">
@@ -5099,17 +5132,17 @@
       <c r="K74" t="s">
         <v>51</v>
       </c>
-      <c r="M74">
-        <v>5</v>
-      </c>
-      <c r="N74">
-        <v>5</v>
+      <c r="M74" t="s">
+        <v>61</v>
+      </c>
+      <c r="N74" t="s">
+        <v>61</v>
       </c>
       <c r="O74" t="s">
+        <v>62</v>
+      </c>
+      <c r="P74" t="s">
         <v>59</v>
-      </c>
-      <c r="P74">
-        <v>1</v>
       </c>
       <c r="Q74" t="s">
         <v>56</v>
@@ -5127,13 +5160,13 @@
         <v>52</v>
       </c>
       <c r="V74" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
       <c r="W74" t="s">
         <v>52</v>
       </c>
       <c r="X74" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
     </row>
     <row r="75" spans="1:24">
@@ -5158,17 +5191,17 @@
       <c r="K75" t="s">
         <v>51</v>
       </c>
-      <c r="M75">
-        <v>5</v>
-      </c>
-      <c r="N75">
-        <v>5</v>
+      <c r="M75" t="s">
+        <v>61</v>
+      </c>
+      <c r="N75" t="s">
+        <v>61</v>
       </c>
       <c r="O75" t="s">
+        <v>62</v>
+      </c>
+      <c r="P75" t="s">
         <v>59</v>
-      </c>
-      <c r="P75">
-        <v>1</v>
       </c>
       <c r="Q75" t="s">
         <v>56</v>
@@ -5187,6 +5220,9 @@
       </c>
       <c r="W75" t="s">
         <v>56</v>
+      </c>
+      <c r="X75" t="s">
+        <v>100</v>
       </c>
     </row>
     <row r="76" spans="1:24">
@@ -5211,17 +5247,17 @@
       <c r="K76" t="s">
         <v>51</v>
       </c>
-      <c r="M76">
-        <v>5</v>
-      </c>
-      <c r="N76">
-        <v>4</v>
+      <c r="M76" t="s">
+        <v>61</v>
+      </c>
+      <c r="N76" t="s">
+        <v>61</v>
       </c>
       <c r="O76" t="s">
+        <v>62</v>
+      </c>
+      <c r="P76" t="s">
         <v>59</v>
-      </c>
-      <c r="P76">
-        <v>1</v>
       </c>
       <c r="Q76" t="s">
         <v>56</v>
@@ -5240,6 +5276,9 @@
       </c>
       <c r="W76" t="s">
         <v>52</v>
+      </c>
+      <c r="X76" t="s">
+        <v>100</v>
       </c>
     </row>
     <row r="77" spans="1:24">
@@ -5267,17 +5306,17 @@
       <c r="K77" t="s">
         <v>51</v>
       </c>
-      <c r="M77">
-        <v>5</v>
-      </c>
-      <c r="N77">
-        <v>5</v>
+      <c r="M77" t="s">
+        <v>61</v>
+      </c>
+      <c r="N77" t="s">
+        <v>61</v>
       </c>
       <c r="O77" t="s">
+        <v>62</v>
+      </c>
+      <c r="P77" t="s">
         <v>59</v>
-      </c>
-      <c r="P77">
-        <v>0</v>
       </c>
       <c r="Q77" t="s">
         <v>56</v>
@@ -5295,10 +5334,13 @@
         <v>56</v>
       </c>
       <c r="V77" t="s">
-        <v>90</v>
+        <v>93</v>
       </c>
       <c r="W77" t="s">
         <v>56</v>
+      </c>
+      <c r="X77" t="s">
+        <v>100</v>
       </c>
     </row>
     <row r="78" spans="1:24">
@@ -5323,17 +5365,17 @@
       <c r="K78" t="s">
         <v>51</v>
       </c>
-      <c r="M78">
-        <v>3</v>
-      </c>
-      <c r="N78">
-        <v>5</v>
+      <c r="M78" t="s">
+        <v>60</v>
+      </c>
+      <c r="N78" t="s">
+        <v>61</v>
       </c>
       <c r="O78" t="s">
-        <v>63</v>
-      </c>
-      <c r="P78">
-        <v>0</v>
+        <v>66</v>
+      </c>
+      <c r="P78" t="s">
+        <v>59</v>
       </c>
       <c r="Q78" t="s">
         <v>56</v>
@@ -5357,7 +5399,7 @@
         <v>52</v>
       </c>
       <c r="X78" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
     </row>
     <row r="79" spans="1:24">
@@ -5382,17 +5424,17 @@
       <c r="K79" t="s">
         <v>51</v>
       </c>
-      <c r="M79">
-        <v>4</v>
-      </c>
-      <c r="N79">
-        <v>5</v>
+      <c r="M79" t="s">
+        <v>61</v>
+      </c>
+      <c r="N79" t="s">
+        <v>61</v>
       </c>
       <c r="O79" t="s">
+        <v>62</v>
+      </c>
+      <c r="P79" t="s">
         <v>59</v>
-      </c>
-      <c r="P79">
-        <v>0</v>
       </c>
       <c r="Q79" t="s">
         <v>56</v>
@@ -5410,10 +5452,13 @@
         <v>52</v>
       </c>
       <c r="V79" t="s">
-        <v>86</v>
+        <v>89</v>
       </c>
       <c r="W79" t="s">
         <v>56</v>
+      </c>
+      <c r="X79" t="s">
+        <v>100</v>
       </c>
     </row>
     <row r="80" spans="1:24">
@@ -5441,17 +5486,17 @@
       <c r="K80" t="s">
         <v>51</v>
       </c>
-      <c r="M80">
-        <v>0</v>
-      </c>
-      <c r="N80">
-        <v>5</v>
+      <c r="M80" t="s">
+        <v>59</v>
+      </c>
+      <c r="N80" t="s">
+        <v>61</v>
       </c>
       <c r="O80" t="s">
+        <v>62</v>
+      </c>
+      <c r="P80" t="s">
         <v>59</v>
-      </c>
-      <c r="P80">
-        <v>1</v>
       </c>
       <c r="Q80" t="s">
         <v>56</v>
@@ -5475,7 +5520,7 @@
         <v>52</v>
       </c>
       <c r="X80" t="s">
-        <v>113</v>
+        <v>103</v>
       </c>
     </row>
     <row r="81" spans="1:24">
@@ -5500,17 +5545,17 @@
       <c r="K81" t="s">
         <v>51</v>
       </c>
-      <c r="M81">
-        <v>2</v>
-      </c>
-      <c r="N81">
-        <v>5</v>
+      <c r="M81" t="s">
+        <v>60</v>
+      </c>
+      <c r="N81" t="s">
+        <v>61</v>
       </c>
       <c r="O81" t="s">
-        <v>62</v>
-      </c>
-      <c r="P81">
-        <v>1</v>
+        <v>65</v>
+      </c>
+      <c r="P81" t="s">
+        <v>59</v>
       </c>
       <c r="Q81" t="s">
         <v>52</v>
@@ -5528,13 +5573,13 @@
         <v>56</v>
       </c>
       <c r="V81" t="s">
-        <v>69</v>
+        <v>72</v>
       </c>
       <c r="W81" t="s">
         <v>52</v>
       </c>
       <c r="X81" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
     </row>
     <row r="82" spans="1:24">
@@ -5562,17 +5607,17 @@
       <c r="K82" t="s">
         <v>51</v>
       </c>
-      <c r="M82">
-        <v>5</v>
-      </c>
-      <c r="N82">
-        <v>2</v>
+      <c r="M82" t="s">
+        <v>61</v>
+      </c>
+      <c r="N82" t="s">
+        <v>60</v>
       </c>
       <c r="O82" t="s">
-        <v>59</v>
-      </c>
-      <c r="P82">
-        <v>5</v>
+        <v>62</v>
+      </c>
+      <c r="P82" t="s">
+        <v>61</v>
       </c>
       <c r="Q82" t="s">
         <v>56</v>
@@ -5590,13 +5635,13 @@
         <v>52</v>
       </c>
       <c r="V82" t="s">
-        <v>91</v>
+        <v>94</v>
       </c>
       <c r="W82" t="s">
         <v>52</v>
       </c>
       <c r="X82" t="s">
-        <v>109</v>
+        <v>101</v>
       </c>
     </row>
     <row r="83" spans="1:24">
@@ -5624,17 +5669,17 @@
       <c r="K83" t="s">
         <v>51</v>
       </c>
-      <c r="M83">
-        <v>3</v>
-      </c>
-      <c r="N83">
-        <v>5</v>
+      <c r="M83" t="s">
+        <v>60</v>
+      </c>
+      <c r="N83" t="s">
+        <v>61</v>
       </c>
       <c r="O83" t="s">
+        <v>62</v>
+      </c>
+      <c r="P83" t="s">
         <v>59</v>
-      </c>
-      <c r="P83">
-        <v>0</v>
       </c>
       <c r="Q83" t="s">
         <v>56</v>
@@ -5652,13 +5697,13 @@
         <v>52</v>
       </c>
       <c r="V83" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="W83" t="s">
         <v>52</v>
       </c>
       <c r="X83" t="s">
-        <v>109</v>
+        <v>101</v>
       </c>
     </row>
     <row r="84" spans="1:24">
@@ -5683,17 +5728,17 @@
       <c r="K84" t="s">
         <v>51</v>
       </c>
-      <c r="M84">
-        <v>4</v>
-      </c>
-      <c r="N84">
-        <v>2</v>
+      <c r="M84" t="s">
+        <v>61</v>
+      </c>
+      <c r="N84" t="s">
+        <v>60</v>
       </c>
       <c r="O84" t="s">
+        <v>62</v>
+      </c>
+      <c r="P84" t="s">
         <v>59</v>
-      </c>
-      <c r="P84">
-        <v>1</v>
       </c>
       <c r="Q84" t="s">
         <v>56</v>
@@ -5711,13 +5756,13 @@
         <v>52</v>
       </c>
       <c r="V84" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
       <c r="W84" t="s">
         <v>52</v>
       </c>
       <c r="X84" t="s">
-        <v>113</v>
+        <v>103</v>
       </c>
     </row>
     <row r="85" spans="1:24">
@@ -5745,17 +5790,17 @@
       <c r="K85" t="s">
         <v>51</v>
       </c>
-      <c r="M85">
-        <v>4</v>
-      </c>
-      <c r="N85">
-        <v>4</v>
+      <c r="M85" t="s">
+        <v>61</v>
+      </c>
+      <c r="N85" t="s">
+        <v>61</v>
       </c>
       <c r="O85" t="s">
+        <v>62</v>
+      </c>
+      <c r="P85" t="s">
         <v>59</v>
-      </c>
-      <c r="P85">
-        <v>0</v>
       </c>
       <c r="Q85" t="s">
         <v>56</v>
@@ -5773,13 +5818,13 @@
         <v>56</v>
       </c>
       <c r="V85" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
       <c r="W85" t="s">
         <v>52</v>
       </c>
       <c r="X85" t="s">
-        <v>109</v>
+        <v>101</v>
       </c>
     </row>
     <row r="86" spans="1:24">
@@ -5804,17 +5849,17 @@
       <c r="K86" t="s">
         <v>51</v>
       </c>
-      <c r="M86">
-        <v>5</v>
-      </c>
-      <c r="N86">
-        <v>2</v>
+      <c r="M86" t="s">
+        <v>61</v>
+      </c>
+      <c r="N86" t="s">
+        <v>60</v>
       </c>
       <c r="O86" t="s">
-        <v>62</v>
-      </c>
-      <c r="P86">
-        <v>0</v>
+        <v>65</v>
+      </c>
+      <c r="P86" t="s">
+        <v>59</v>
       </c>
       <c r="Q86" t="s">
         <v>56</v>
@@ -5832,13 +5877,13 @@
         <v>56</v>
       </c>
       <c r="V86" t="s">
-        <v>86</v>
+        <v>89</v>
       </c>
       <c r="W86" t="s">
         <v>52</v>
       </c>
       <c r="X86" t="s">
-        <v>109</v>
+        <v>101</v>
       </c>
     </row>
     <row r="87" spans="1:24">
@@ -5863,17 +5908,17 @@
       <c r="K87" t="s">
         <v>51</v>
       </c>
-      <c r="M87">
-        <v>5</v>
-      </c>
-      <c r="N87">
-        <v>5</v>
+      <c r="M87" t="s">
+        <v>61</v>
+      </c>
+      <c r="N87" t="s">
+        <v>61</v>
       </c>
       <c r="O87" t="s">
-        <v>59</v>
-      </c>
-      <c r="P87">
-        <v>5</v>
+        <v>62</v>
+      </c>
+      <c r="P87" t="s">
+        <v>61</v>
       </c>
       <c r="Q87" t="s">
         <v>52</v>
@@ -5897,7 +5942,7 @@
         <v>52</v>
       </c>
       <c r="X87" t="s">
-        <v>109</v>
+        <v>101</v>
       </c>
     </row>
     <row r="88" spans="1:24">
@@ -5922,17 +5967,17 @@
       <c r="K88" t="s">
         <v>51</v>
       </c>
-      <c r="M88">
-        <v>3</v>
-      </c>
-      <c r="N88">
-        <v>5</v>
+      <c r="M88" t="s">
+        <v>60</v>
+      </c>
+      <c r="N88" t="s">
+        <v>61</v>
       </c>
       <c r="O88" t="s">
+        <v>62</v>
+      </c>
+      <c r="P88" t="s">
         <v>59</v>
-      </c>
-      <c r="P88">
-        <v>0</v>
       </c>
       <c r="Q88" t="s">
         <v>56</v>
@@ -5950,10 +5995,13 @@
         <v>52</v>
       </c>
       <c r="V88" t="s">
-        <v>92</v>
+        <v>95</v>
       </c>
       <c r="W88" t="s">
         <v>56</v>
+      </c>
+      <c r="X88" t="s">
+        <v>100</v>
       </c>
     </row>
     <row r="89" spans="1:24">
@@ -5978,17 +6026,17 @@
       <c r="K89" t="s">
         <v>51</v>
       </c>
-      <c r="M89">
-        <v>5</v>
-      </c>
-      <c r="N89">
-        <v>4</v>
+      <c r="M89" t="s">
+        <v>61</v>
+      </c>
+      <c r="N89" t="s">
+        <v>61</v>
       </c>
       <c r="O89" t="s">
-        <v>59</v>
-      </c>
-      <c r="P89">
-        <v>3</v>
+        <v>62</v>
+      </c>
+      <c r="P89" t="s">
+        <v>60</v>
       </c>
       <c r="Q89" t="s">
         <v>52</v>
@@ -6010,6 +6058,9 @@
       </c>
       <c r="W89" t="s">
         <v>56</v>
+      </c>
+      <c r="X89" t="s">
+        <v>100</v>
       </c>
     </row>
     <row r="90" spans="1:24">
@@ -6037,17 +6088,17 @@
       <c r="K90" t="s">
         <v>51</v>
       </c>
-      <c r="M90">
-        <v>2</v>
-      </c>
-      <c r="N90">
-        <v>5</v>
+      <c r="M90" t="s">
+        <v>60</v>
+      </c>
+      <c r="N90" t="s">
+        <v>61</v>
       </c>
       <c r="O90" t="s">
-        <v>59</v>
-      </c>
-      <c r="P90">
-        <v>2</v>
+        <v>62</v>
+      </c>
+      <c r="P90" t="s">
+        <v>60</v>
       </c>
       <c r="Q90" t="s">
         <v>56</v>
@@ -6065,10 +6116,13 @@
         <v>52</v>
       </c>
       <c r="V90" t="s">
-        <v>90</v>
+        <v>93</v>
       </c>
       <c r="W90" t="s">
         <v>56</v>
+      </c>
+      <c r="X90" t="s">
+        <v>100</v>
       </c>
     </row>
     <row r="91" spans="1:24">
@@ -6096,17 +6150,17 @@
       <c r="K91" t="s">
         <v>51</v>
       </c>
-      <c r="M91">
-        <v>5</v>
-      </c>
-      <c r="N91">
-        <v>4</v>
+      <c r="M91" t="s">
+        <v>61</v>
+      </c>
+      <c r="N91" t="s">
+        <v>61</v>
       </c>
       <c r="O91" t="s">
+        <v>62</v>
+      </c>
+      <c r="P91" t="s">
         <v>59</v>
-      </c>
-      <c r="P91">
-        <v>0</v>
       </c>
       <c r="Q91" t="s">
         <v>56</v>
@@ -6124,13 +6178,13 @@
         <v>56</v>
       </c>
       <c r="V91" t="s">
-        <v>85</v>
+        <v>88</v>
       </c>
       <c r="W91" t="s">
         <v>52</v>
       </c>
       <c r="X91" t="s">
-        <v>113</v>
+        <v>103</v>
       </c>
     </row>
     <row r="92" spans="1:24">
@@ -6155,17 +6209,17 @@
       <c r="K92" t="s">
         <v>51</v>
       </c>
-      <c r="M92">
-        <v>2</v>
-      </c>
-      <c r="N92">
-        <v>5</v>
+      <c r="M92" t="s">
+        <v>60</v>
+      </c>
+      <c r="N92" t="s">
+        <v>61</v>
       </c>
       <c r="O92" t="s">
+        <v>62</v>
+      </c>
+      <c r="P92" t="s">
         <v>59</v>
-      </c>
-      <c r="P92">
-        <v>0</v>
       </c>
       <c r="Q92" t="s">
         <v>56</v>
@@ -6183,13 +6237,13 @@
         <v>56</v>
       </c>
       <c r="V92" t="s">
-        <v>72</v>
+        <v>75</v>
       </c>
       <c r="W92" t="s">
         <v>52</v>
       </c>
       <c r="X92" t="s">
-        <v>109</v>
+        <v>101</v>
       </c>
     </row>
     <row r="93" spans="1:24">
@@ -6226,17 +6280,17 @@
       <c r="K93" t="s">
         <v>51</v>
       </c>
-      <c r="M93">
-        <v>5</v>
-      </c>
-      <c r="N93">
-        <v>3</v>
+      <c r="M93" t="s">
+        <v>61</v>
+      </c>
+      <c r="N93" t="s">
+        <v>60</v>
       </c>
       <c r="O93" t="s">
-        <v>59</v>
-      </c>
-      <c r="P93">
-        <v>2</v>
+        <v>62</v>
+      </c>
+      <c r="P93" t="s">
+        <v>60</v>
       </c>
       <c r="Q93" t="s">
         <v>56</v>
@@ -6254,13 +6308,13 @@
         <v>56</v>
       </c>
       <c r="V93" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
       <c r="W93" t="s">
         <v>52</v>
       </c>
       <c r="X93" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
     </row>
     <row r="94" spans="1:24">
@@ -6288,17 +6342,17 @@
       <c r="L94" t="s">
         <v>58</v>
       </c>
-      <c r="M94">
-        <v>1</v>
-      </c>
-      <c r="N94">
-        <v>4</v>
+      <c r="M94" t="s">
+        <v>59</v>
+      </c>
+      <c r="N94" t="s">
+        <v>61</v>
       </c>
       <c r="O94" t="s">
+        <v>62</v>
+      </c>
+      <c r="P94" t="s">
         <v>59</v>
-      </c>
-      <c r="P94">
-        <v>0</v>
       </c>
       <c r="Q94" t="s">
         <v>56</v>
@@ -6319,7 +6373,7 @@
         <v>52</v>
       </c>
       <c r="X94" t="s">
-        <v>115</v>
+        <v>99</v>
       </c>
     </row>
     <row r="95" spans="1:24">
@@ -6347,17 +6401,17 @@
       <c r="K95" t="s">
         <v>51</v>
       </c>
-      <c r="M95">
-        <v>1</v>
-      </c>
-      <c r="N95">
-        <v>5</v>
+      <c r="M95" t="s">
+        <v>59</v>
+      </c>
+      <c r="N95" t="s">
+        <v>61</v>
       </c>
       <c r="O95" t="s">
-        <v>59</v>
-      </c>
-      <c r="P95">
-        <v>2</v>
+        <v>62</v>
+      </c>
+      <c r="P95" t="s">
+        <v>60</v>
       </c>
       <c r="Q95" t="s">
         <v>56</v>
@@ -6375,13 +6429,13 @@
         <v>56</v>
       </c>
       <c r="V95" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
       <c r="W95" t="s">
         <v>52</v>
       </c>
       <c r="X95" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
     </row>
     <row r="96" spans="1:24">
@@ -6406,17 +6460,17 @@
       <c r="K96" t="s">
         <v>51</v>
       </c>
-      <c r="M96">
-        <v>5</v>
-      </c>
-      <c r="N96">
-        <v>2</v>
+      <c r="M96" t="s">
+        <v>61</v>
+      </c>
+      <c r="N96" t="s">
+        <v>60</v>
       </c>
       <c r="O96" t="s">
-        <v>62</v>
-      </c>
-      <c r="P96">
-        <v>0</v>
+        <v>65</v>
+      </c>
+      <c r="P96" t="s">
+        <v>59</v>
       </c>
       <c r="Q96" t="s">
         <v>56</v>
@@ -6434,13 +6488,13 @@
         <v>56</v>
       </c>
       <c r="V96" t="s">
-        <v>86</v>
+        <v>89</v>
       </c>
       <c r="W96" t="s">
         <v>52</v>
       </c>
       <c r="X96" t="s">
-        <v>109</v>
+        <v>101</v>
       </c>
     </row>
     <row r="97" spans="1:24">
@@ -6465,17 +6519,17 @@
       <c r="K97" t="s">
         <v>51</v>
       </c>
-      <c r="M97">
-        <v>3</v>
-      </c>
-      <c r="N97">
-        <v>5</v>
+      <c r="M97" t="s">
+        <v>60</v>
+      </c>
+      <c r="N97" t="s">
+        <v>61</v>
       </c>
       <c r="O97" t="s">
+        <v>62</v>
+      </c>
+      <c r="P97" t="s">
         <v>59</v>
-      </c>
-      <c r="P97">
-        <v>1</v>
       </c>
       <c r="Q97" t="s">
         <v>56</v>
@@ -6493,10 +6547,13 @@
         <v>56</v>
       </c>
       <c r="V97" t="s">
-        <v>91</v>
+        <v>94</v>
       </c>
       <c r="W97" t="s">
         <v>56</v>
+      </c>
+      <c r="X97" t="s">
+        <v>100</v>
       </c>
     </row>
     <row r="98" spans="1:24">
@@ -6521,17 +6578,17 @@
       <c r="K98" t="s">
         <v>51</v>
       </c>
-      <c r="M98">
-        <v>5</v>
-      </c>
-      <c r="N98">
-        <v>5</v>
+      <c r="M98" t="s">
+        <v>61</v>
+      </c>
+      <c r="N98" t="s">
+        <v>61</v>
       </c>
       <c r="O98" t="s">
-        <v>59</v>
-      </c>
-      <c r="P98">
-        <v>5</v>
+        <v>62</v>
+      </c>
+      <c r="P98" t="s">
+        <v>61</v>
       </c>
       <c r="Q98" t="s">
         <v>52</v>
@@ -6549,10 +6606,13 @@
         <v>52</v>
       </c>
       <c r="V98" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="W98" t="s">
         <v>56</v>
+      </c>
+      <c r="X98" t="s">
+        <v>100</v>
       </c>
     </row>
     <row r="99" spans="1:24">
@@ -6580,17 +6640,17 @@
       <c r="K99" t="s">
         <v>51</v>
       </c>
-      <c r="M99">
-        <v>3</v>
-      </c>
-      <c r="N99">
-        <v>4</v>
+      <c r="M99" t="s">
+        <v>60</v>
+      </c>
+      <c r="N99" t="s">
+        <v>61</v>
       </c>
       <c r="O99" t="s">
-        <v>62</v>
-      </c>
-      <c r="P99">
-        <v>0</v>
+        <v>65</v>
+      </c>
+      <c r="P99" t="s">
+        <v>59</v>
       </c>
       <c r="Q99" t="s">
         <v>56</v>
@@ -6609,6 +6669,9 @@
       </c>
       <c r="W99" t="s">
         <v>56</v>
+      </c>
+      <c r="X99" t="s">
+        <v>100</v>
       </c>
     </row>
     <row r="100" spans="1:24">
@@ -6633,17 +6696,17 @@
       <c r="K100" t="s">
         <v>51</v>
       </c>
-      <c r="M100">
-        <v>3</v>
-      </c>
-      <c r="N100">
-        <v>2</v>
+      <c r="M100" t="s">
+        <v>60</v>
+      </c>
+      <c r="N100" t="s">
+        <v>60</v>
       </c>
       <c r="O100" t="s">
+        <v>62</v>
+      </c>
+      <c r="P100" t="s">
         <v>59</v>
-      </c>
-      <c r="P100">
-        <v>0</v>
       </c>
       <c r="Q100" t="s">
         <v>56</v>
@@ -6661,13 +6724,13 @@
         <v>56</v>
       </c>
       <c r="V100" t="s">
-        <v>93</v>
+        <v>96</v>
       </c>
       <c r="W100" t="s">
         <v>52</v>
       </c>
       <c r="X100" t="s">
-        <v>109</v>
+        <v>101</v>
       </c>
     </row>
     <row r="101" spans="1:24">
@@ -6692,17 +6755,17 @@
       <c r="K101" t="s">
         <v>51</v>
       </c>
-      <c r="M101">
-        <v>2</v>
-      </c>
-      <c r="N101">
-        <v>4</v>
+      <c r="M101" t="s">
+        <v>60</v>
+      </c>
+      <c r="N101" t="s">
+        <v>61</v>
       </c>
       <c r="O101" t="s">
+        <v>62</v>
+      </c>
+      <c r="P101" t="s">
         <v>59</v>
-      </c>
-      <c r="P101">
-        <v>0</v>
       </c>
       <c r="Q101" t="s">
         <v>56</v>
@@ -6720,13 +6783,13 @@
         <v>56</v>
       </c>
       <c r="V101" t="s">
-        <v>94</v>
+        <v>97</v>
       </c>
       <c r="W101" t="s">
         <v>52</v>
       </c>
       <c r="X101" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
     </row>
     <row r="102" spans="1:24">
@@ -6754,17 +6817,17 @@
       <c r="K102" t="s">
         <v>51</v>
       </c>
-      <c r="M102">
-        <v>2</v>
-      </c>
-      <c r="N102">
-        <v>4</v>
+      <c r="M102" t="s">
+        <v>60</v>
+      </c>
+      <c r="N102" t="s">
+        <v>61</v>
       </c>
       <c r="O102" t="s">
+        <v>62</v>
+      </c>
+      <c r="P102" t="s">
         <v>59</v>
-      </c>
-      <c r="P102">
-        <v>1</v>
       </c>
       <c r="Q102" t="s">
         <v>56</v>
@@ -6788,7 +6851,7 @@
         <v>52</v>
       </c>
       <c r="X102" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
     </row>
     <row r="103" spans="1:24">
@@ -6828,17 +6891,17 @@
       <c r="L103" t="s">
         <v>58</v>
       </c>
-      <c r="M103">
-        <v>2</v>
-      </c>
-      <c r="N103">
-        <v>3</v>
+      <c r="M103" t="s">
+        <v>60</v>
+      </c>
+      <c r="N103" t="s">
+        <v>60</v>
       </c>
       <c r="O103" t="s">
-        <v>59</v>
-      </c>
-      <c r="P103">
-        <v>4</v>
+        <v>62</v>
+      </c>
+      <c r="P103" t="s">
+        <v>61</v>
       </c>
       <c r="Q103" t="s">
         <v>52</v>
@@ -6860,6 +6923,9 @@
       </c>
       <c r="W103" t="s">
         <v>56</v>
+      </c>
+      <c r="X103" t="s">
+        <v>100</v>
       </c>
     </row>
     <row r="104" spans="1:24">
@@ -6887,17 +6953,17 @@
       <c r="K104" t="s">
         <v>51</v>
       </c>
-      <c r="M104">
-        <v>4</v>
-      </c>
-      <c r="N104">
-        <v>4</v>
+      <c r="M104" t="s">
+        <v>61</v>
+      </c>
+      <c r="N104" t="s">
+        <v>61</v>
       </c>
       <c r="O104" t="s">
-        <v>59</v>
-      </c>
-      <c r="P104">
-        <v>3</v>
+        <v>62</v>
+      </c>
+      <c r="P104" t="s">
+        <v>60</v>
       </c>
       <c r="Q104" t="s">
         <v>56</v>
@@ -6915,10 +6981,13 @@
         <v>52</v>
       </c>
       <c r="V104" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
       <c r="W104" t="s">
         <v>56</v>
+      </c>
+      <c r="X104" t="s">
+        <v>100</v>
       </c>
     </row>
     <row r="105" spans="1:24">
@@ -6946,17 +7015,17 @@
       <c r="K105" t="s">
         <v>51</v>
       </c>
-      <c r="M105">
-        <v>3</v>
-      </c>
-      <c r="N105">
-        <v>5</v>
+      <c r="M105" t="s">
+        <v>60</v>
+      </c>
+      <c r="N105" t="s">
+        <v>61</v>
       </c>
       <c r="O105" t="s">
-        <v>62</v>
-      </c>
-      <c r="P105">
-        <v>2</v>
+        <v>65</v>
+      </c>
+      <c r="P105" t="s">
+        <v>60</v>
       </c>
       <c r="Q105" t="s">
         <v>56</v>
@@ -6977,7 +7046,7 @@
         <v>52</v>
       </c>
       <c r="X105" t="s">
-        <v>109</v>
+        <v>101</v>
       </c>
     </row>
     <row r="106" spans="1:24">
@@ -7002,17 +7071,17 @@
       <c r="K106" t="s">
         <v>51</v>
       </c>
-      <c r="M106">
-        <v>2</v>
-      </c>
-      <c r="N106">
-        <v>5</v>
+      <c r="M106" t="s">
+        <v>60</v>
+      </c>
+      <c r="N106" t="s">
+        <v>61</v>
       </c>
       <c r="O106" t="s">
-        <v>59</v>
-      </c>
-      <c r="P106">
-        <v>4</v>
+        <v>62</v>
+      </c>
+      <c r="P106" t="s">
+        <v>61</v>
       </c>
       <c r="Q106" t="s">
         <v>52</v>
@@ -7030,13 +7099,13 @@
         <v>52</v>
       </c>
       <c r="V106" t="s">
-        <v>95</v>
+        <v>98</v>
       </c>
       <c r="W106" t="s">
         <v>52</v>
       </c>
       <c r="X106" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
     </row>
     <row r="107" spans="1:24">
@@ -7061,17 +7130,17 @@
       <c r="K107" t="s">
         <v>51</v>
       </c>
-      <c r="M107">
-        <v>3</v>
-      </c>
-      <c r="N107">
-        <v>2</v>
+      <c r="M107" t="s">
+        <v>60</v>
+      </c>
+      <c r="N107" t="s">
+        <v>60</v>
       </c>
       <c r="O107" t="s">
+        <v>62</v>
+      </c>
+      <c r="P107" t="s">
         <v>59</v>
-      </c>
-      <c r="P107">
-        <v>0</v>
       </c>
       <c r="Q107" t="s">
         <v>56</v>
@@ -7095,7 +7164,7 @@
         <v>52</v>
       </c>
       <c r="X107" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add color blindness toggle
</commit_message>
<xml_diff>
--- a/data-cleaning/cleaned.xlsx
+++ b/data-cleaning/cleaned.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1955" uniqueCount="108">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1955" uniqueCount="106">
   <si>
     <t>sexe</t>
   </si>
@@ -205,13 +205,13 @@
     <t>1 fois par mois</t>
   </si>
   <si>
-    <t>rarement 0-1 fois/semaine</t>
-  </si>
-  <si>
-    <t>occasionnellement 2-3 fois/semaine</t>
-  </si>
-  <si>
-    <t>Fréquente &gt;4 fois/semaine</t>
+    <t>rarement</t>
+  </si>
+  <si>
+    <t>occasionnellement</t>
+  </si>
+  <si>
+    <t>Fréquente</t>
   </si>
   <si>
     <t>Huile végétale</t>
@@ -220,13 +220,7 @@
     <t>Zit ziton</t>
   </si>
   <si>
-    <t>Beurre ou beurre allégé</t>
-  </si>
-  <si>
-    <t>Margarine</t>
-  </si>
-  <si>
-    <t>Margarine et huile végétale</t>
+    <t>Beurre</t>
   </si>
   <si>
     <t>8</t>
@@ -822,13 +816,13 @@
         <v>60</v>
       </c>
       <c r="V2" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="W2" t="s">
         <v>56</v>
       </c>
       <c r="X2" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
     </row>
     <row r="3" spans="1:24">
@@ -890,13 +884,13 @@
         <v>56</v>
       </c>
       <c r="V3" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="W3" t="s">
         <v>60</v>
       </c>
       <c r="X3" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
     </row>
     <row r="4" spans="1:24">
@@ -955,13 +949,13 @@
         <v>60</v>
       </c>
       <c r="V4" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="W4" t="s">
         <v>56</v>
       </c>
       <c r="X4" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
     </row>
     <row r="5" spans="1:24">
@@ -1023,13 +1017,13 @@
         <v>60</v>
       </c>
       <c r="V5" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="W5" t="s">
         <v>60</v>
       </c>
       <c r="X5" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
     </row>
     <row r="6" spans="1:24">
@@ -1082,13 +1076,13 @@
         <v>56</v>
       </c>
       <c r="V6" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="W6" t="s">
         <v>60</v>
       </c>
       <c r="X6" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
     </row>
     <row r="7" spans="1:24">
@@ -1138,13 +1132,13 @@
         <v>60</v>
       </c>
       <c r="V7" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="W7" t="s">
         <v>56</v>
       </c>
       <c r="X7" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
     </row>
     <row r="8" spans="1:24">
@@ -1200,7 +1194,7 @@
         <v>60</v>
       </c>
       <c r="X8" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
     </row>
     <row r="9" spans="1:24">
@@ -1256,13 +1250,13 @@
         <v>60</v>
       </c>
       <c r="V9" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="W9" t="s">
         <v>56</v>
       </c>
       <c r="X9" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="10" spans="1:24">
@@ -1318,13 +1312,13 @@
         <v>60</v>
       </c>
       <c r="V10" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="W10" t="s">
         <v>56</v>
       </c>
       <c r="X10" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="11" spans="1:24">
@@ -1356,7 +1350,7 @@
         <v>65</v>
       </c>
       <c r="O11" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="P11" t="s">
         <v>64</v>
@@ -1383,7 +1377,7 @@
         <v>56</v>
       </c>
       <c r="X11" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
     </row>
     <row r="12" spans="1:24">
@@ -1439,7 +1433,7 @@
         <v>60</v>
       </c>
       <c r="X12" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
     </row>
     <row r="13" spans="1:24">
@@ -1495,7 +1489,7 @@
         <v>60</v>
       </c>
       <c r="X13" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
     </row>
     <row r="14" spans="1:24">
@@ -1545,13 +1539,13 @@
         <v>56</v>
       </c>
       <c r="V14" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="W14" t="s">
         <v>60</v>
       </c>
       <c r="X14" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
     </row>
     <row r="15" spans="1:24">
@@ -1580,7 +1574,7 @@
         <v>64</v>
       </c>
       <c r="O15" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="P15" t="s">
         <v>64</v>
@@ -1601,13 +1595,13 @@
         <v>60</v>
       </c>
       <c r="V15" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="W15" t="s">
         <v>56</v>
       </c>
       <c r="X15" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
     </row>
     <row r="16" spans="1:24">
@@ -1663,13 +1657,13 @@
         <v>60</v>
       </c>
       <c r="V16" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="W16" t="s">
         <v>56</v>
       </c>
       <c r="X16" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="17" spans="1:24">
@@ -1719,13 +1713,13 @@
         <v>60</v>
       </c>
       <c r="V17" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="W17" t="s">
         <v>56</v>
       </c>
       <c r="X17" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
     </row>
     <row r="18" spans="1:24">
@@ -1787,13 +1781,13 @@
         <v>56</v>
       </c>
       <c r="V18" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="W18" t="s">
         <v>56</v>
       </c>
       <c r="X18" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
     </row>
     <row r="19" spans="1:24">
@@ -1846,13 +1840,13 @@
         <v>56</v>
       </c>
       <c r="V19" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="W19" t="s">
         <v>56</v>
       </c>
       <c r="X19" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="20" spans="1:24">
@@ -1908,7 +1902,7 @@
         <v>56</v>
       </c>
       <c r="X20" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
     </row>
     <row r="21" spans="1:24">
@@ -1964,7 +1958,7 @@
         <v>56</v>
       </c>
       <c r="X21" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
     </row>
     <row r="22" spans="1:24">
@@ -2029,7 +2023,7 @@
         <v>56</v>
       </c>
       <c r="X22" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
     </row>
     <row r="23" spans="1:24">
@@ -2085,7 +2079,7 @@
         <v>60</v>
       </c>
       <c r="X23" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
     </row>
     <row r="24" spans="1:24">
@@ -2135,13 +2129,13 @@
         <v>56</v>
       </c>
       <c r="V24" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="W24" t="s">
         <v>56</v>
       </c>
       <c r="X24" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
     </row>
     <row r="25" spans="1:24">
@@ -2200,7 +2194,7 @@
         <v>60</v>
       </c>
       <c r="X25" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
     </row>
     <row r="26" spans="1:24">
@@ -2253,13 +2247,13 @@
         <v>60</v>
       </c>
       <c r="V26" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="W26" t="s">
         <v>60</v>
       </c>
       <c r="X26" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
     </row>
     <row r="27" spans="1:24">
@@ -2309,13 +2303,13 @@
         <v>56</v>
       </c>
       <c r="V27" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="W27" t="s">
         <v>60</v>
       </c>
       <c r="X27" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
     </row>
     <row r="28" spans="1:24">
@@ -2377,7 +2371,7 @@
         <v>56</v>
       </c>
       <c r="X28" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="29" spans="1:24">
@@ -2436,13 +2430,13 @@
         <v>60</v>
       </c>
       <c r="V29" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="W29" t="s">
         <v>56</v>
       </c>
       <c r="X29" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="30" spans="1:24">
@@ -2495,13 +2489,13 @@
         <v>60</v>
       </c>
       <c r="V30" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="W30" t="s">
         <v>56</v>
       </c>
       <c r="X30" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
     </row>
     <row r="31" spans="1:24">
@@ -2557,13 +2551,13 @@
         <v>56</v>
       </c>
       <c r="V31" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="W31" t="s">
         <v>56</v>
       </c>
       <c r="X31" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
     </row>
     <row r="32" spans="1:24">
@@ -2628,13 +2622,13 @@
         <v>60</v>
       </c>
       <c r="V32" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="W32" t="s">
         <v>56</v>
       </c>
       <c r="X32" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
     </row>
     <row r="33" spans="1:24">
@@ -2699,13 +2693,13 @@
         <v>60</v>
       </c>
       <c r="V33" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="W33" t="s">
         <v>56</v>
       </c>
       <c r="X33" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="34" spans="1:24">
@@ -2761,7 +2755,7 @@
         <v>60</v>
       </c>
       <c r="X34" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
     </row>
     <row r="35" spans="1:24">
@@ -2820,7 +2814,7 @@
         <v>56</v>
       </c>
       <c r="X35" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
     </row>
     <row r="36" spans="1:24">
@@ -2873,13 +2867,13 @@
         <v>56</v>
       </c>
       <c r="V36" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="W36" t="s">
         <v>56</v>
       </c>
       <c r="X36" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
     </row>
     <row r="37" spans="1:24">
@@ -2932,13 +2926,13 @@
         <v>60</v>
       </c>
       <c r="V37" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="W37" t="s">
         <v>56</v>
       </c>
       <c r="X37" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
     </row>
     <row r="38" spans="1:24">
@@ -2994,13 +2988,13 @@
         <v>60</v>
       </c>
       <c r="V38" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="W38" t="s">
         <v>56</v>
       </c>
       <c r="X38" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
     </row>
     <row r="39" spans="1:24">
@@ -3056,13 +3050,13 @@
         <v>60</v>
       </c>
       <c r="V39" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="W39" t="s">
         <v>60</v>
       </c>
       <c r="X39" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
     </row>
     <row r="40" spans="1:24">
@@ -3124,7 +3118,7 @@
         <v>56</v>
       </c>
       <c r="X40" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
     </row>
     <row r="41" spans="1:24">
@@ -3189,7 +3183,7 @@
         <v>56</v>
       </c>
       <c r="X41" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
     </row>
     <row r="42" spans="1:24">
@@ -3245,13 +3239,13 @@
         <v>60</v>
       </c>
       <c r="V42" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="W42" t="s">
         <v>56</v>
       </c>
       <c r="X42" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="43" spans="1:24">
@@ -3310,7 +3304,7 @@
         <v>56</v>
       </c>
       <c r="X43" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
     </row>
     <row r="44" spans="1:24">
@@ -3366,13 +3360,13 @@
         <v>60</v>
       </c>
       <c r="V44" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="W44" t="s">
         <v>56</v>
       </c>
       <c r="X44" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
     </row>
     <row r="45" spans="1:24">
@@ -3431,7 +3425,7 @@
         <v>56</v>
       </c>
       <c r="X45" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="46" spans="1:24">
@@ -3499,7 +3493,7 @@
         <v>60</v>
       </c>
       <c r="X46" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
     </row>
     <row r="47" spans="1:24">
@@ -3555,7 +3549,7 @@
         <v>56</v>
       </c>
       <c r="X47" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
     </row>
     <row r="48" spans="1:24">
@@ -3608,13 +3602,13 @@
         <v>56</v>
       </c>
       <c r="V48" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="W48" t="s">
         <v>60</v>
       </c>
       <c r="X48" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
     </row>
     <row r="49" spans="1:24">
@@ -3679,13 +3673,13 @@
         <v>60</v>
       </c>
       <c r="V49" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="W49" t="s">
         <v>56</v>
       </c>
       <c r="X49" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="50" spans="1:24">
@@ -3744,7 +3738,7 @@
         <v>60</v>
       </c>
       <c r="X50" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
     </row>
     <row r="51" spans="1:24">
@@ -3809,13 +3803,13 @@
         <v>60</v>
       </c>
       <c r="V51" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="W51" t="s">
         <v>56</v>
       </c>
       <c r="X51" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
     </row>
     <row r="52" spans="1:24">
@@ -3868,13 +3862,13 @@
         <v>60</v>
       </c>
       <c r="V52" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="W52" t="s">
         <v>56</v>
       </c>
       <c r="X52" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="53" spans="1:24">
@@ -3933,7 +3927,7 @@
         <v>60</v>
       </c>
       <c r="X53" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
     </row>
     <row r="54" spans="1:24">
@@ -3986,13 +3980,13 @@
         <v>60</v>
       </c>
       <c r="V54" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="W54" t="s">
         <v>56</v>
       </c>
       <c r="X54" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="55" spans="1:24">
@@ -4054,7 +4048,7 @@
         <v>56</v>
       </c>
       <c r="X55" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="56" spans="1:24">
@@ -4107,13 +4101,13 @@
         <v>60</v>
       </c>
       <c r="V56" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="W56" t="s">
         <v>56</v>
       </c>
       <c r="X56" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
     </row>
     <row r="57" spans="1:24">
@@ -4166,13 +4160,13 @@
         <v>60</v>
       </c>
       <c r="V57" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="W57" t="s">
         <v>56</v>
       </c>
       <c r="X57" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
     </row>
     <row r="58" spans="1:24">
@@ -4225,13 +4219,13 @@
         <v>56</v>
       </c>
       <c r="V58" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="W58" t="s">
         <v>56</v>
       </c>
       <c r="X58" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
     </row>
     <row r="59" spans="1:24">
@@ -4284,13 +4278,13 @@
         <v>60</v>
       </c>
       <c r="V59" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="W59" t="s">
         <v>60</v>
       </c>
       <c r="X59" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
     </row>
     <row r="60" spans="1:24">
@@ -4343,13 +4337,13 @@
         <v>60</v>
       </c>
       <c r="V60" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="W60" t="s">
         <v>56</v>
       </c>
       <c r="X60" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
     </row>
     <row r="61" spans="1:24">
@@ -4408,7 +4402,7 @@
         <v>60</v>
       </c>
       <c r="X61" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
     </row>
     <row r="62" spans="1:24">
@@ -4467,7 +4461,7 @@
         <v>56</v>
       </c>
       <c r="X62" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="63" spans="1:24">
@@ -4523,13 +4517,13 @@
         <v>60</v>
       </c>
       <c r="V63" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="W63" t="s">
         <v>56</v>
       </c>
       <c r="X63" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
     </row>
     <row r="64" spans="1:24">
@@ -4582,13 +4576,13 @@
         <v>56</v>
       </c>
       <c r="V64" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="W64" t="s">
         <v>56</v>
       </c>
       <c r="X64" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
     </row>
     <row r="65" spans="1:24">
@@ -4647,7 +4641,7 @@
         <v>56</v>
       </c>
       <c r="X65" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="66" spans="1:24">
@@ -4706,7 +4700,7 @@
         <v>56</v>
       </c>
       <c r="X66" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
     </row>
     <row r="67" spans="1:24">
@@ -4762,7 +4756,7 @@
         <v>56</v>
       </c>
       <c r="X67" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
     </row>
     <row r="68" spans="1:24">
@@ -4818,7 +4812,7 @@
         <v>56</v>
       </c>
       <c r="X68" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
     </row>
     <row r="69" spans="1:24">
@@ -4871,13 +4865,13 @@
         <v>60</v>
       </c>
       <c r="V69" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="W69" t="s">
         <v>56</v>
       </c>
       <c r="X69" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
     </row>
     <row r="70" spans="1:24">
@@ -4936,13 +4930,13 @@
         <v>56</v>
       </c>
       <c r="V70" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="W70" t="s">
         <v>60</v>
       </c>
       <c r="X70" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
     </row>
     <row r="71" spans="1:24">
@@ -4998,13 +4992,13 @@
         <v>60</v>
       </c>
       <c r="V71" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="W71" t="s">
         <v>56</v>
       </c>
       <c r="X71" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="72" spans="1:24">
@@ -5063,7 +5057,7 @@
         <v>60</v>
       </c>
       <c r="X72" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
     </row>
     <row r="73" spans="1:24">
@@ -5122,7 +5116,7 @@
         <v>56</v>
       </c>
       <c r="X73" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="74" spans="1:24">
@@ -5175,13 +5169,13 @@
         <v>56</v>
       </c>
       <c r="V74" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="W74" t="s">
         <v>56</v>
       </c>
       <c r="X74" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="75" spans="1:24">
@@ -5237,7 +5231,7 @@
         <v>60</v>
       </c>
       <c r="X75" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
     </row>
     <row r="76" spans="1:24">
@@ -5293,7 +5287,7 @@
         <v>56</v>
       </c>
       <c r="X76" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
     </row>
     <row r="77" spans="1:24">
@@ -5349,13 +5343,13 @@
         <v>60</v>
       </c>
       <c r="V77" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="W77" t="s">
         <v>60</v>
       </c>
       <c r="X77" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
     </row>
     <row r="78" spans="1:24">
@@ -5387,7 +5381,7 @@
         <v>65</v>
       </c>
       <c r="O78" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="P78" t="s">
         <v>63</v>
@@ -5414,7 +5408,7 @@
         <v>56</v>
       </c>
       <c r="X78" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="79" spans="1:24">
@@ -5467,13 +5461,13 @@
         <v>56</v>
       </c>
       <c r="V79" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="W79" t="s">
         <v>60</v>
       </c>
       <c r="X79" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
     </row>
     <row r="80" spans="1:24">
@@ -5535,7 +5529,7 @@
         <v>56</v>
       </c>
       <c r="X80" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
     </row>
     <row r="81" spans="1:24">
@@ -5567,7 +5561,7 @@
         <v>65</v>
       </c>
       <c r="O81" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="P81" t="s">
         <v>63</v>
@@ -5588,13 +5582,13 @@
         <v>60</v>
       </c>
       <c r="V81" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="W81" t="s">
         <v>56</v>
       </c>
       <c r="X81" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="82" spans="1:24">
@@ -5650,13 +5644,13 @@
         <v>56</v>
       </c>
       <c r="V82" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="W82" t="s">
         <v>56</v>
       </c>
       <c r="X82" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
     </row>
     <row r="83" spans="1:24">
@@ -5712,13 +5706,13 @@
         <v>56</v>
       </c>
       <c r="V83" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="W83" t="s">
         <v>56</v>
       </c>
       <c r="X83" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
     </row>
     <row r="84" spans="1:24">
@@ -5771,13 +5765,13 @@
         <v>56</v>
       </c>
       <c r="V84" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="W84" t="s">
         <v>56</v>
       </c>
       <c r="X84" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
     </row>
     <row r="85" spans="1:24">
@@ -5833,13 +5827,13 @@
         <v>60</v>
       </c>
       <c r="V85" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="W85" t="s">
         <v>56</v>
       </c>
       <c r="X85" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
     </row>
     <row r="86" spans="1:24">
@@ -5871,7 +5865,7 @@
         <v>64</v>
       </c>
       <c r="O86" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="P86" t="s">
         <v>63</v>
@@ -5892,13 +5886,13 @@
         <v>60</v>
       </c>
       <c r="V86" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="W86" t="s">
         <v>56</v>
       </c>
       <c r="X86" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
     </row>
     <row r="87" spans="1:24">
@@ -5957,7 +5951,7 @@
         <v>56</v>
       </c>
       <c r="X87" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
     </row>
     <row r="88" spans="1:24">
@@ -6010,13 +6004,13 @@
         <v>56</v>
       </c>
       <c r="V88" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="W88" t="s">
         <v>60</v>
       </c>
       <c r="X88" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
     </row>
     <row r="89" spans="1:24">
@@ -6075,7 +6069,7 @@
         <v>60</v>
       </c>
       <c r="X89" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
     </row>
     <row r="90" spans="1:24">
@@ -6131,13 +6125,13 @@
         <v>56</v>
       </c>
       <c r="V90" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="W90" t="s">
         <v>60</v>
       </c>
       <c r="X90" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
     </row>
     <row r="91" spans="1:24">
@@ -6193,13 +6187,13 @@
         <v>60</v>
       </c>
       <c r="V91" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="W91" t="s">
         <v>56</v>
       </c>
       <c r="X91" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
     </row>
     <row r="92" spans="1:24">
@@ -6252,13 +6246,13 @@
         <v>60</v>
       </c>
       <c r="V92" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="W92" t="s">
         <v>56</v>
       </c>
       <c r="X92" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
     </row>
     <row r="93" spans="1:24">
@@ -6323,13 +6317,13 @@
         <v>60</v>
       </c>
       <c r="V93" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="W93" t="s">
         <v>56</v>
       </c>
       <c r="X93" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="94" spans="1:24">
@@ -6388,7 +6382,7 @@
         <v>56</v>
       </c>
       <c r="X94" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
     </row>
     <row r="95" spans="1:24">
@@ -6444,13 +6438,13 @@
         <v>60</v>
       </c>
       <c r="V95" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="W95" t="s">
         <v>56</v>
       </c>
       <c r="X95" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="96" spans="1:24">
@@ -6482,7 +6476,7 @@
         <v>64</v>
       </c>
       <c r="O96" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="P96" t="s">
         <v>63</v>
@@ -6503,13 +6497,13 @@
         <v>60</v>
       </c>
       <c r="V96" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="W96" t="s">
         <v>56</v>
       </c>
       <c r="X96" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
     </row>
     <row r="97" spans="1:24">
@@ -6562,13 +6556,13 @@
         <v>60</v>
       </c>
       <c r="V97" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="W97" t="s">
         <v>60</v>
       </c>
       <c r="X97" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
     </row>
     <row r="98" spans="1:24">
@@ -6621,13 +6615,13 @@
         <v>56</v>
       </c>
       <c r="V98" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="W98" t="s">
         <v>60</v>
       </c>
       <c r="X98" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
     </row>
     <row r="99" spans="1:24">
@@ -6662,7 +6656,7 @@
         <v>65</v>
       </c>
       <c r="O99" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="P99" t="s">
         <v>63</v>
@@ -6686,7 +6680,7 @@
         <v>60</v>
       </c>
       <c r="X99" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
     </row>
     <row r="100" spans="1:24">
@@ -6739,13 +6733,13 @@
         <v>60</v>
       </c>
       <c r="V100" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="W100" t="s">
         <v>56</v>
       </c>
       <c r="X100" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
     </row>
     <row r="101" spans="1:24">
@@ -6798,13 +6792,13 @@
         <v>60</v>
       </c>
       <c r="V101" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="W101" t="s">
         <v>56</v>
       </c>
       <c r="X101" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="102" spans="1:24">
@@ -6866,7 +6860,7 @@
         <v>56</v>
       </c>
       <c r="X102" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="103" spans="1:24">
@@ -6940,7 +6934,7 @@
         <v>60</v>
       </c>
       <c r="X103" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
     </row>
     <row r="104" spans="1:24">
@@ -6996,13 +6990,13 @@
         <v>56</v>
       </c>
       <c r="V104" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="W104" t="s">
         <v>60</v>
       </c>
       <c r="X104" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
     </row>
     <row r="105" spans="1:24">
@@ -7037,7 +7031,7 @@
         <v>65</v>
       </c>
       <c r="O105" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="P105" t="s">
         <v>64</v>
@@ -7061,7 +7055,7 @@
         <v>56</v>
       </c>
       <c r="X105" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
     </row>
     <row r="106" spans="1:24">
@@ -7114,13 +7108,13 @@
         <v>56</v>
       </c>
       <c r="V106" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="W106" t="s">
         <v>56</v>
       </c>
       <c r="X106" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="107" spans="1:24">
@@ -7179,7 +7173,7 @@
         <v>56</v>
       </c>
       <c r="X107" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
onHover add colors according to sexe
</commit_message>
<xml_diff>
--- a/data-cleaning/cleaned.xlsx
+++ b/data-cleaning/cleaned.xlsx
@@ -205,13 +205,13 @@
     <t>1 fois par mois</t>
   </si>
   <si>
-    <t>rarement</t>
-  </si>
-  <si>
-    <t>occasionnellement</t>
-  </si>
-  <si>
-    <t>Fréquente</t>
+    <t>Rarely</t>
+  </si>
+  <si>
+    <t>Occasionally</t>
+  </si>
+  <si>
+    <t>Frequently</t>
   </si>
   <si>
     <t>Huile végétale</t>
@@ -319,19 +319,19 @@
     <t>1</t>
   </si>
   <si>
-    <t>autres</t>
-  </si>
-  <si>
-    <t>aucune maladie</t>
-  </si>
-  <si>
-    <t>diabete</t>
-  </si>
-  <si>
-    <t>HTA</t>
-  </si>
-  <si>
-    <t>asthme</t>
+    <t>Others</t>
+  </si>
+  <si>
+    <t>None</t>
+  </si>
+  <si>
+    <t>Diabetes</t>
+  </si>
+  <si>
+    <t>Hypertension</t>
+  </si>
+  <si>
+    <t>Asthma</t>
   </si>
 </sst>
 </file>

</xml_diff>